<commit_message>
Varios cambios introducidos, el word estaba corrupto y se ha tenido que realizar un trabajo de recomposicion. Ademas, se aumenta el tamanio de las notas de las imagenes de resultados.
</commit_message>
<xml_diff>
--- a/code/v7/Resultados.xlsx
+++ b/code/v7/Resultados.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Cristian\Downloads\deteccion de fraude\v7\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Cristian\Documents\5- Educación\6- Master Universitario en Big Data y Ciencias de Datos\2- Asignaturas\12. TFM\2. Entregable\code\v7\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F9C417B-8E06-42EE-B8C5-97D91050447D}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1219E2D0-5F2E-471C-ACD6-8787A043B0CE}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="12510" activeTab="3" xr2:uid="{9BF040E8-FE20-4374-BDF1-F7EE73AA9256}"/>
   </bookViews>
@@ -131,7 +131,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="169" formatCode="0.000"/>
+    <numFmt numFmtId="164" formatCode="0.000"/>
   </numFmts>
   <fonts count="4" x14ac:knownFonts="1">
     <font>
@@ -371,7 +371,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -380,22 +380,10 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="169" fontId="1" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="1" fontId="1" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="1" fontId="1" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="169" fontId="1" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="1" fontId="1" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="1" fontId="1" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
@@ -425,6 +413,19 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -772,563 +773,563 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" s="1" customFormat="1" ht="44.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="20" t="s">
+      <c r="A1" s="16" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="21" t="s">
+      <c r="B1" s="17" t="s">
         <v>22</v>
       </c>
       <c r="C1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="21" t="s">
+      <c r="D1" s="17" t="s">
         <v>23</v>
       </c>
-      <c r="E1" s="21" t="s">
+      <c r="E1" s="17" t="s">
         <v>24</v>
       </c>
-      <c r="F1" s="21" t="s">
+      <c r="F1" s="17" t="s">
         <v>25</v>
       </c>
-      <c r="G1" s="21" t="s">
+      <c r="G1" s="17" t="s">
         <v>19</v>
       </c>
-      <c r="H1" s="21" t="s">
+      <c r="H1" s="17" t="s">
         <v>18</v>
       </c>
-      <c r="I1" s="21" t="s">
+      <c r="I1" s="17" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="21" t="s">
+      <c r="J1" s="17" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="21" t="s">
+      <c r="K1" s="17" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="21" t="s">
+      <c r="L1" s="17" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="21" t="s">
+      <c r="M1" s="17" t="s">
         <v>26</v>
       </c>
-      <c r="N1" s="22" t="s">
+      <c r="N1" s="18" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A2" s="23">
+      <c r="A2" s="19">
         <v>1</v>
       </c>
-      <c r="B2" s="24" t="s">
-        <v>17</v>
-      </c>
-      <c r="C2" s="25" t="s">
+      <c r="B2" s="20" t="s">
+        <v>17</v>
+      </c>
+      <c r="C2" s="21" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="24" t="s">
-        <v>13</v>
-      </c>
-      <c r="E2" s="24" t="s">
-        <v>13</v>
-      </c>
-      <c r="F2" s="24" t="s">
-        <v>14</v>
-      </c>
-      <c r="G2" s="24">
+      <c r="D2" s="20" t="s">
+        <v>13</v>
+      </c>
+      <c r="E2" s="20" t="s">
+        <v>13</v>
+      </c>
+      <c r="F2" s="20" t="s">
+        <v>14</v>
+      </c>
+      <c r="G2" s="20">
         <v>0</v>
       </c>
-      <c r="H2" s="24">
+      <c r="H2" s="20">
         <v>0.79600000000000004</v>
       </c>
-      <c r="I2" s="24">
+      <c r="I2" s="20">
         <v>0.04</v>
       </c>
-      <c r="J2" s="24">
+      <c r="J2" s="20">
         <v>5.3999999999999999E-2</v>
       </c>
-      <c r="K2" s="24">
+      <c r="K2" s="20">
         <v>0.78700000000000003</v>
       </c>
-      <c r="L2" s="24">
+      <c r="L2" s="20">
         <v>0.80300000000000005</v>
       </c>
-      <c r="M2" s="24">
+      <c r="M2" s="20">
         <v>339</v>
       </c>
-      <c r="N2" s="26">
+      <c r="N2" s="22">
         <v>5909</v>
       </c>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A3" s="17">
+      <c r="A3" s="13">
         <v>2</v>
       </c>
-      <c r="B3" s="18" t="s">
+      <c r="B3" s="14" t="s">
         <v>17</v>
       </c>
       <c r="C3" s="2"/>
-      <c r="D3" s="18" t="s">
-        <v>13</v>
-      </c>
-      <c r="E3" s="18" t="s">
-        <v>13</v>
-      </c>
-      <c r="F3" s="18" t="s">
-        <v>14</v>
-      </c>
-      <c r="G3" s="18">
+      <c r="D3" s="14" t="s">
+        <v>13</v>
+      </c>
+      <c r="E3" s="14" t="s">
+        <v>13</v>
+      </c>
+      <c r="F3" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="G3" s="14">
         <v>0.33</v>
       </c>
-      <c r="H3" s="18">
+      <c r="H3" s="14">
         <v>0.79900000000000004</v>
       </c>
-      <c r="I3" s="18">
+      <c r="I3" s="14">
         <v>0.04</v>
       </c>
-      <c r="J3" s="18">
+      <c r="J3" s="14">
         <v>5.6000000000000001E-2</v>
       </c>
-      <c r="K3" s="18">
+      <c r="K3" s="14">
         <v>0.78900000000000003</v>
       </c>
-      <c r="L3" s="18">
+      <c r="L3" s="14">
         <v>0.80900000000000005</v>
       </c>
-      <c r="M3" s="18">
+      <c r="M3" s="14">
         <v>340</v>
       </c>
-      <c r="N3" s="19">
+      <c r="N3" s="15">
         <v>5771</v>
       </c>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A4" s="17">
+      <c r="A4" s="13">
         <v>3</v>
       </c>
-      <c r="B4" s="18" t="s">
+      <c r="B4" s="14" t="s">
         <v>17</v>
       </c>
       <c r="C4" s="2"/>
-      <c r="D4" s="18" t="s">
-        <v>13</v>
-      </c>
-      <c r="E4" s="18" t="s">
-        <v>13</v>
-      </c>
-      <c r="F4" s="18" t="s">
-        <v>14</v>
-      </c>
-      <c r="G4" s="18">
+      <c r="D4" s="14" t="s">
+        <v>13</v>
+      </c>
+      <c r="E4" s="14" t="s">
+        <v>13</v>
+      </c>
+      <c r="F4" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="G4" s="14">
         <v>0.5</v>
       </c>
-      <c r="H4" s="18">
+      <c r="H4" s="14">
         <v>0.80200000000000005</v>
       </c>
-      <c r="I4" s="18">
+      <c r="I4" s="14">
         <v>0.02</v>
       </c>
-      <c r="J4" s="18">
+      <c r="J4" s="14">
         <v>4.9000000000000002E-2</v>
       </c>
-      <c r="K4" s="18">
+      <c r="K4" s="14">
         <v>0.83299999999999996</v>
       </c>
-      <c r="L4" s="18">
+      <c r="L4" s="14">
         <v>0.77200000000000002</v>
       </c>
-      <c r="M4" s="18">
+      <c r="M4" s="14">
         <v>359</v>
       </c>
-      <c r="N4" s="19">
+      <c r="N4" s="15">
         <v>6948</v>
       </c>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A5" s="17">
+      <c r="A5" s="13">
         <v>4</v>
       </c>
-      <c r="B5" s="18" t="s">
+      <c r="B5" s="14" t="s">
         <v>17</v>
       </c>
       <c r="C5" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="D5" s="18" t="s">
-        <v>12</v>
-      </c>
-      <c r="E5" s="18" t="s">
-        <v>13</v>
-      </c>
-      <c r="F5" s="18" t="s">
-        <v>14</v>
-      </c>
-      <c r="G5" s="18">
+      <c r="D5" s="14" t="s">
+        <v>12</v>
+      </c>
+      <c r="E5" s="14" t="s">
+        <v>13</v>
+      </c>
+      <c r="F5" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="G5" s="14">
         <v>0</v>
       </c>
-      <c r="H5" s="18">
+      <c r="H5" s="14">
         <v>0.77100000000000002</v>
       </c>
-      <c r="I5" s="18">
+      <c r="I5" s="14">
         <v>0.2</v>
       </c>
-      <c r="J5" s="18">
+      <c r="J5" s="14">
         <v>4.7E-2</v>
       </c>
-      <c r="K5" s="18">
+      <c r="K5" s="14">
         <v>0.76300000000000001</v>
       </c>
-      <c r="L5" s="18">
+      <c r="L5" s="14">
         <v>0.77800000000000002</v>
       </c>
-      <c r="M5" s="18">
+      <c r="M5" s="14">
         <v>329</v>
       </c>
-      <c r="N5" s="19">
+      <c r="N5" s="15">
         <v>6728</v>
       </c>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A6" s="17">
+      <c r="A6" s="13">
         <v>5</v>
       </c>
-      <c r="B6" s="18" t="s">
+      <c r="B6" s="14" t="s">
         <v>17</v>
       </c>
       <c r="C6" s="2"/>
-      <c r="D6" s="18" t="s">
-        <v>12</v>
-      </c>
-      <c r="E6" s="18" t="s">
-        <v>13</v>
-      </c>
-      <c r="F6" s="18" t="s">
-        <v>14</v>
-      </c>
-      <c r="G6" s="18">
+      <c r="D6" s="14" t="s">
+        <v>12</v>
+      </c>
+      <c r="E6" s="14" t="s">
+        <v>13</v>
+      </c>
+      <c r="F6" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="G6" s="14">
         <v>0.33</v>
       </c>
-      <c r="H6" s="18">
+      <c r="H6" s="14">
         <v>0.80700000000000005</v>
       </c>
-      <c r="I6" s="18">
+      <c r="I6" s="14">
         <v>0.42</v>
       </c>
-      <c r="J6" s="18">
+      <c r="J6" s="14">
         <v>5.5E-2</v>
       </c>
-      <c r="K6" s="18">
+      <c r="K6" s="14">
         <v>0.81399999999999995</v>
       </c>
-      <c r="L6" s="18">
+      <c r="L6" s="14">
         <v>0.8</v>
       </c>
-      <c r="M6" s="18">
+      <c r="M6" s="14">
         <v>351</v>
       </c>
-      <c r="N6" s="19">
+      <c r="N6" s="15">
         <v>6082</v>
       </c>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A7" s="17">
+      <c r="A7" s="13">
         <v>6</v>
       </c>
-      <c r="B7" s="18" t="s">
+      <c r="B7" s="14" t="s">
         <v>17</v>
       </c>
       <c r="C7" s="2"/>
-      <c r="D7" s="18" t="s">
-        <v>12</v>
-      </c>
-      <c r="E7" s="18" t="s">
-        <v>13</v>
-      </c>
-      <c r="F7" s="18" t="s">
-        <v>14</v>
-      </c>
-      <c r="G7" s="18">
+      <c r="D7" s="14" t="s">
+        <v>12</v>
+      </c>
+      <c r="E7" s="14" t="s">
+        <v>13</v>
+      </c>
+      <c r="F7" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="G7" s="14">
         <v>0.5</v>
       </c>
-      <c r="H7" s="18">
+      <c r="H7" s="14">
         <v>0.81100000000000005</v>
       </c>
-      <c r="I7" s="18">
+      <c r="I7" s="14">
         <v>0.43</v>
       </c>
-      <c r="J7" s="18">
+      <c r="J7" s="14">
         <v>5.5E-2</v>
       </c>
-      <c r="K7" s="18">
+      <c r="K7" s="14">
         <v>0.82399999999999995</v>
       </c>
-      <c r="L7" s="18">
+      <c r="L7" s="14">
         <v>0.8</v>
       </c>
-      <c r="M7" s="18">
+      <c r="M7" s="14">
         <v>355</v>
       </c>
-      <c r="N7" s="19">
+      <c r="N7" s="15">
         <v>6089</v>
       </c>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A8" s="17">
+      <c r="A8" s="13">
         <v>7</v>
       </c>
-      <c r="B8" s="18" t="s">
+      <c r="B8" s="14" t="s">
         <v>17</v>
       </c>
       <c r="C8" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="D8" s="18" t="s">
-        <v>12</v>
-      </c>
-      <c r="E8" s="18" t="s">
-        <v>12</v>
-      </c>
-      <c r="F8" s="18" t="s">
+      <c r="D8" s="14" t="s">
+        <v>12</v>
+      </c>
+      <c r="E8" s="14" t="s">
+        <v>12</v>
+      </c>
+      <c r="F8" s="14" t="s">
         <v>15</v>
       </c>
-      <c r="G8" s="18">
+      <c r="G8" s="14">
         <v>0</v>
       </c>
-      <c r="H8" s="18">
+      <c r="H8" s="14">
         <v>0.78700000000000003</v>
       </c>
-      <c r="I8" s="18">
+      <c r="I8" s="14">
         <v>0.19</v>
       </c>
-      <c r="J8" s="18">
+      <c r="J8" s="14">
         <v>5.1999999999999998E-2</v>
       </c>
-      <c r="K8" s="18">
+      <c r="K8" s="14">
         <v>0.77500000000000002</v>
       </c>
-      <c r="L8" s="18">
+      <c r="L8" s="14">
         <v>0.79800000000000004</v>
       </c>
-      <c r="M8" s="18">
+      <c r="M8" s="14">
         <v>334</v>
       </c>
-      <c r="N8" s="19">
+      <c r="N8" s="15">
         <v>6109</v>
       </c>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A9" s="17">
+      <c r="A9" s="13">
         <v>8</v>
       </c>
-      <c r="B9" s="18" t="s">
+      <c r="B9" s="14" t="s">
         <v>17</v>
       </c>
       <c r="C9" s="2"/>
-      <c r="D9" s="18" t="s">
-        <v>12</v>
-      </c>
-      <c r="E9" s="18" t="s">
-        <v>12</v>
-      </c>
-      <c r="F9" s="18" t="s">
+      <c r="D9" s="14" t="s">
+        <v>12</v>
+      </c>
+      <c r="E9" s="14" t="s">
+        <v>12</v>
+      </c>
+      <c r="F9" s="14" t="s">
         <v>15</v>
       </c>
-      <c r="G9" s="18">
+      <c r="G9" s="14">
         <v>0.33</v>
       </c>
-      <c r="H9" s="18">
+      <c r="H9" s="14">
         <v>0.79400000000000004</v>
       </c>
-      <c r="I9" s="18">
+      <c r="I9" s="14">
         <v>0.37</v>
       </c>
-      <c r="J9" s="18">
+      <c r="J9" s="14">
         <v>4.8000000000000001E-2</v>
       </c>
-      <c r="K9" s="18">
+      <c r="K9" s="14">
         <v>0.82099999999999995</v>
       </c>
-      <c r="L9" s="18">
+      <c r="L9" s="14">
         <v>0.76800000000000002</v>
       </c>
-      <c r="M9" s="18">
+      <c r="M9" s="14">
         <v>354</v>
       </c>
-      <c r="N9" s="19">
+      <c r="N9" s="15">
         <v>7050</v>
       </c>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A10" s="17">
+      <c r="A10" s="13">
         <v>9</v>
       </c>
-      <c r="B10" s="18" t="s">
+      <c r="B10" s="14" t="s">
         <v>17</v>
       </c>
       <c r="C10" s="2"/>
-      <c r="D10" s="18" t="s">
-        <v>12</v>
-      </c>
-      <c r="E10" s="18" t="s">
-        <v>12</v>
-      </c>
-      <c r="F10" s="18" t="s">
+      <c r="D10" s="14" t="s">
+        <v>12</v>
+      </c>
+      <c r="E10" s="14" t="s">
+        <v>12</v>
+      </c>
+      <c r="F10" s="14" t="s">
         <v>15</v>
       </c>
-      <c r="G10" s="18">
+      <c r="G10" s="14">
         <v>0.5</v>
       </c>
-      <c r="H10" s="18">
+      <c r="H10" s="14">
         <v>0.80400000000000005</v>
       </c>
-      <c r="I10" s="18">
+      <c r="I10" s="14">
         <v>0.43</v>
       </c>
-      <c r="J10" s="18">
+      <c r="J10" s="14">
         <v>6.0999999999999999E-2</v>
       </c>
-      <c r="K10" s="18">
+      <c r="K10" s="14">
         <v>0.78</v>
       </c>
-      <c r="L10" s="18">
+      <c r="L10" s="14">
         <v>0.82699999999999996</v>
       </c>
-      <c r="M10" s="18">
+      <c r="M10" s="14">
         <v>336</v>
       </c>
-      <c r="N10" s="19">
+      <c r="N10" s="15">
         <v>5211</v>
       </c>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A11" s="17">
+      <c r="A11" s="13">
         <v>10</v>
       </c>
-      <c r="B11" s="18" t="s">
+      <c r="B11" s="14" t="s">
         <v>17</v>
       </c>
       <c r="C11" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="D11" s="18" t="s">
-        <v>12</v>
-      </c>
-      <c r="E11" s="18" t="s">
-        <v>12</v>
-      </c>
-      <c r="F11" s="18" t="s">
+      <c r="D11" s="14" t="s">
+        <v>12</v>
+      </c>
+      <c r="E11" s="14" t="s">
+        <v>12</v>
+      </c>
+      <c r="F11" s="14" t="s">
         <v>16</v>
       </c>
-      <c r="G11" s="18">
+      <c r="G11" s="14">
         <v>0</v>
       </c>
-      <c r="H11" s="18">
+      <c r="H11" s="14">
         <v>0.76600000000000001</v>
       </c>
-      <c r="I11" s="18">
+      <c r="I11" s="14">
         <v>0.03</v>
       </c>
-      <c r="J11" s="18">
+      <c r="J11" s="14">
         <v>4.9000000000000002E-2</v>
       </c>
-      <c r="K11" s="18">
+      <c r="K11" s="14">
         <v>0.73299999999999998</v>
       </c>
-      <c r="L11" s="18">
+      <c r="L11" s="14">
         <v>0.79900000000000004</v>
       </c>
-      <c r="M11" s="18">
+      <c r="M11" s="14">
         <v>316</v>
       </c>
-      <c r="N11" s="19">
+      <c r="N11" s="15">
         <v>6071</v>
       </c>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A12" s="17">
+      <c r="A12" s="13">
         <v>11</v>
       </c>
-      <c r="B12" s="18" t="s">
+      <c r="B12" s="14" t="s">
         <v>17</v>
       </c>
       <c r="C12" s="2"/>
-      <c r="D12" s="18" t="s">
-        <v>12</v>
-      </c>
-      <c r="E12" s="18" t="s">
-        <v>12</v>
-      </c>
-      <c r="F12" s="18" t="s">
+      <c r="D12" s="14" t="s">
+        <v>12</v>
+      </c>
+      <c r="E12" s="14" t="s">
+        <v>12</v>
+      </c>
+      <c r="F12" s="14" t="s">
         <v>16</v>
       </c>
-      <c r="G12" s="18">
+      <c r="G12" s="14">
         <v>0.33</v>
       </c>
-      <c r="H12" s="18">
+      <c r="H12" s="14">
         <v>0.80400000000000005</v>
       </c>
-      <c r="I12" s="18">
+      <c r="I12" s="14">
         <v>0.41</v>
       </c>
-      <c r="J12" s="18">
+      <c r="J12" s="14">
         <v>5.2999999999999999E-2</v>
       </c>
-      <c r="K12" s="18">
+      <c r="K12" s="14">
         <v>0.81699999999999995</v>
       </c>
-      <c r="L12" s="18">
+      <c r="L12" s="14">
         <v>0.79200000000000004</v>
       </c>
-      <c r="M12" s="18">
+      <c r="M12" s="14">
         <v>352</v>
       </c>
-      <c r="N12" s="19">
+      <c r="N12" s="15">
         <v>6310</v>
       </c>
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A13" s="17">
-        <v>12</v>
-      </c>
-      <c r="B13" s="18" t="s">
+      <c r="A13" s="13">
+        <v>12</v>
+      </c>
+      <c r="B13" s="14" t="s">
         <v>17</v>
       </c>
       <c r="C13" s="2"/>
-      <c r="D13" s="18" t="s">
-        <v>12</v>
-      </c>
-      <c r="E13" s="18" t="s">
-        <v>12</v>
-      </c>
-      <c r="F13" s="18" t="s">
+      <c r="D13" s="14" t="s">
+        <v>12</v>
+      </c>
+      <c r="E13" s="14" t="s">
+        <v>12</v>
+      </c>
+      <c r="F13" s="14" t="s">
         <v>16</v>
       </c>
-      <c r="G13" s="18">
+      <c r="G13" s="14">
         <v>0.5</v>
       </c>
-      <c r="H13" s="18">
+      <c r="H13" s="14">
         <v>0.80700000000000005</v>
       </c>
-      <c r="I13" s="18">
+      <c r="I13" s="14">
         <v>0.48</v>
       </c>
-      <c r="J13" s="18">
+      <c r="J13" s="14">
         <v>0.06</v>
       </c>
-      <c r="K13" s="18">
+      <c r="K13" s="14">
         <v>0.78900000000000003</v>
       </c>
-      <c r="L13" s="18">
+      <c r="L13" s="14">
         <v>0.82499999999999996</v>
       </c>
-      <c r="M13" s="18">
+      <c r="M13" s="14">
         <v>340</v>
       </c>
-      <c r="N13" s="19">
+      <c r="N13" s="15">
         <v>5298</v>
       </c>
     </row>
     <row r="14" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="14">
+      <c r="A14" s="10">
         <v>13</v>
       </c>
       <c r="B14" s="2" t="s">
@@ -1367,12 +1368,12 @@
       <c r="M14" s="2">
         <v>337</v>
       </c>
-      <c r="N14" s="15">
+      <c r="N14" s="11">
         <v>7231</v>
       </c>
     </row>
     <row r="15" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="14">
+      <c r="A15" s="10">
         <v>14</v>
       </c>
       <c r="B15" s="2" t="s">
@@ -1409,12 +1410,12 @@
       <c r="M15" s="2">
         <v>339</v>
       </c>
-      <c r="N15" s="15">
+      <c r="N15" s="11">
         <v>7101</v>
       </c>
     </row>
     <row r="16" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="14">
+      <c r="A16" s="10">
         <v>15</v>
       </c>
       <c r="B16" s="2" t="s">
@@ -1451,15 +1452,15 @@
       <c r="M16" s="2">
         <v>349</v>
       </c>
-      <c r="N16" s="15">
+      <c r="N16" s="11">
         <v>5882</v>
       </c>
     </row>
     <row r="17" spans="1:14" ht="75" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="14">
+      <c r="A17" s="10">
         <v>18</v>
       </c>
-      <c r="B17" s="16" t="s">
+      <c r="B17" s="12" t="s">
         <v>28</v>
       </c>
       <c r="C17" s="2"/>
@@ -1493,126 +1494,126 @@
       <c r="M17" s="2">
         <v>351</v>
       </c>
-      <c r="N17" s="15">
+      <c r="N17" s="11">
         <v>6426</v>
       </c>
     </row>
     <row r="18" spans="1:14" ht="60.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="27">
+      <c r="A18" s="23">
         <v>21</v>
       </c>
-      <c r="B18" s="28" t="s">
+      <c r="B18" s="24" t="s">
         <v>29</v>
       </c>
-      <c r="C18" s="29"/>
-      <c r="D18" s="29" t="s">
-        <v>12</v>
-      </c>
-      <c r="E18" s="29" t="s">
-        <v>13</v>
-      </c>
-      <c r="F18" s="29" t="s">
-        <v>14</v>
-      </c>
-      <c r="G18" s="29">
+      <c r="C18" s="25"/>
+      <c r="D18" s="25" t="s">
+        <v>12</v>
+      </c>
+      <c r="E18" s="25" t="s">
+        <v>13</v>
+      </c>
+      <c r="F18" s="25" t="s">
+        <v>14</v>
+      </c>
+      <c r="G18" s="25">
         <v>0.5</v>
       </c>
-      <c r="H18" s="29">
+      <c r="H18" s="25">
         <v>0.81299999999999994</v>
       </c>
-      <c r="I18" s="29">
+      <c r="I18" s="25">
         <v>0.46</v>
       </c>
-      <c r="J18" s="29">
+      <c r="J18" s="25">
         <v>6.0999999999999999E-2</v>
       </c>
-      <c r="K18" s="29">
+      <c r="K18" s="25">
         <v>0.8</v>
       </c>
-      <c r="L18" s="29">
+      <c r="L18" s="25">
         <v>0.82399999999999995</v>
       </c>
-      <c r="M18" s="29">
+      <c r="M18" s="25">
         <v>345</v>
       </c>
-      <c r="N18" s="30">
+      <c r="N18" s="26">
         <v>5314</v>
       </c>
     </row>
     <row r="19" spans="1:14" ht="20.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="4" t="s">
+      <c r="A19" s="27" t="s">
         <v>20</v>
       </c>
-      <c r="B19" s="5"/>
-      <c r="C19" s="5"/>
-      <c r="D19" s="5"/>
-      <c r="E19" s="5"/>
-      <c r="F19" s="5"/>
-      <c r="G19" s="5"/>
-      <c r="H19" s="6">
+      <c r="B19" s="28"/>
+      <c r="C19" s="28"/>
+      <c r="D19" s="28"/>
+      <c r="E19" s="28"/>
+      <c r="F19" s="28"/>
+      <c r="G19" s="28"/>
+      <c r="H19" s="4">
         <f>AVERAGE(H2:H18)</f>
         <v>0.79517647058823548</v>
       </c>
-      <c r="I19" s="6">
+      <c r="I19" s="4">
         <f t="shared" ref="I19:N19" si="0">AVERAGE(I2:I18)</f>
         <v>0.30352941176470588</v>
       </c>
-      <c r="J19" s="6">
+      <c r="J19" s="4">
         <f t="shared" si="0"/>
         <v>5.2882352941176484E-2</v>
       </c>
-      <c r="K19" s="6">
+      <c r="K19" s="4">
         <f t="shared" si="0"/>
         <v>0.79517647058823537</v>
       </c>
-      <c r="L19" s="6">
+      <c r="L19" s="4">
         <f t="shared" si="0"/>
         <v>0.79170588235294126</v>
       </c>
-      <c r="M19" s="7">
+      <c r="M19" s="5">
         <f t="shared" si="0"/>
         <v>342.70588235294116</v>
       </c>
-      <c r="N19" s="8">
+      <c r="N19" s="6">
         <f t="shared" si="0"/>
         <v>6207.6470588235297</v>
       </c>
     </row>
     <row r="20" spans="1:14" ht="19.5" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="9" t="s">
+      <c r="A20" s="29" t="s">
         <v>21</v>
       </c>
-      <c r="B20" s="10"/>
-      <c r="C20" s="10"/>
-      <c r="D20" s="10"/>
-      <c r="E20" s="10"/>
-      <c r="F20" s="10"/>
-      <c r="G20" s="10"/>
-      <c r="H20" s="11">
+      <c r="B20" s="30"/>
+      <c r="C20" s="30"/>
+      <c r="D20" s="30"/>
+      <c r="E20" s="30"/>
+      <c r="F20" s="30"/>
+      <c r="G20" s="30"/>
+      <c r="H20" s="7">
         <f>_xlfn.STDEV.P(H2:H18)</f>
         <v>1.4697880175756631E-2</v>
       </c>
-      <c r="I20" s="11">
+      <c r="I20" s="7">
         <f t="shared" ref="I20:N20" si="1">_xlfn.STDEV.P(I2:I18)</f>
         <v>0.17931048250157627</v>
       </c>
-      <c r="J20" s="11">
+      <c r="J20" s="7">
         <f t="shared" si="1"/>
         <v>4.9215295678475025E-3</v>
       </c>
-      <c r="K20" s="11">
+      <c r="K20" s="7">
         <f t="shared" si="1"/>
         <v>2.4588938914784763E-2</v>
       </c>
-      <c r="L20" s="11">
+      <c r="L20" s="7">
         <f t="shared" si="1"/>
         <v>2.7970077931882331E-2</v>
       </c>
-      <c r="M20" s="12">
+      <c r="M20" s="8">
         <f t="shared" si="1"/>
         <v>10.598361171217508</v>
       </c>
-      <c r="N20" s="13">
+      <c r="N20" s="9">
         <f t="shared" si="1"/>
         <v>618.13123879456407</v>
       </c>
@@ -1746,563 +1747,563 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" s="1" customFormat="1" ht="44.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="20" t="s">
+      <c r="A1" s="16" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="21" t="s">
+      <c r="B1" s="17" t="s">
         <v>22</v>
       </c>
       <c r="C1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="21" t="s">
+      <c r="D1" s="17" t="s">
         <v>23</v>
       </c>
-      <c r="E1" s="21" t="s">
+      <c r="E1" s="17" t="s">
         <v>24</v>
       </c>
-      <c r="F1" s="21" t="s">
+      <c r="F1" s="17" t="s">
         <v>25</v>
       </c>
-      <c r="G1" s="21" t="s">
+      <c r="G1" s="17" t="s">
         <v>19</v>
       </c>
-      <c r="H1" s="21" t="s">
+      <c r="H1" s="17" t="s">
         <v>18</v>
       </c>
-      <c r="I1" s="21" t="s">
+      <c r="I1" s="17" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="21" t="s">
+      <c r="J1" s="17" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="21" t="s">
+      <c r="K1" s="17" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="21" t="s">
+      <c r="L1" s="17" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="21" t="s">
+      <c r="M1" s="17" t="s">
         <v>26</v>
       </c>
-      <c r="N1" s="22" t="s">
+      <c r="N1" s="18" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="2" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="23">
+      <c r="A2" s="19">
         <v>1</v>
       </c>
-      <c r="B2" s="24" t="s">
-        <v>17</v>
-      </c>
-      <c r="C2" s="25" t="s">
+      <c r="B2" s="20" t="s">
+        <v>17</v>
+      </c>
+      <c r="C2" s="21" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="24" t="s">
-        <v>13</v>
-      </c>
-      <c r="E2" s="24" t="s">
-        <v>13</v>
-      </c>
-      <c r="F2" s="24" t="s">
-        <v>14</v>
-      </c>
-      <c r="G2" s="24">
+      <c r="D2" s="20" t="s">
+        <v>13</v>
+      </c>
+      <c r="E2" s="20" t="s">
+        <v>13</v>
+      </c>
+      <c r="F2" s="20" t="s">
+        <v>14</v>
+      </c>
+      <c r="G2" s="20">
         <v>0</v>
       </c>
-      <c r="H2" s="24">
+      <c r="H2" s="20">
         <v>0.79600000000000004</v>
       </c>
-      <c r="I2" s="24">
+      <c r="I2" s="20">
         <v>0.04</v>
       </c>
-      <c r="J2" s="24">
+      <c r="J2" s="20">
         <v>5.3999999999999999E-2</v>
       </c>
-      <c r="K2" s="24">
+      <c r="K2" s="20">
         <v>0.78700000000000003</v>
       </c>
-      <c r="L2" s="24">
+      <c r="L2" s="20">
         <v>0.80300000000000005</v>
       </c>
-      <c r="M2" s="24">
+      <c r="M2" s="20">
         <v>339</v>
       </c>
-      <c r="N2" s="26">
+      <c r="N2" s="22">
         <v>5909</v>
       </c>
     </row>
     <row r="3" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="17">
+      <c r="A3" s="13">
         <v>2</v>
       </c>
-      <c r="B3" s="18" t="s">
+      <c r="B3" s="14" t="s">
         <v>17</v>
       </c>
       <c r="C3" s="2"/>
-      <c r="D3" s="18" t="s">
-        <v>13</v>
-      </c>
-      <c r="E3" s="18" t="s">
-        <v>13</v>
-      </c>
-      <c r="F3" s="18" t="s">
-        <v>14</v>
-      </c>
-      <c r="G3" s="18">
+      <c r="D3" s="14" t="s">
+        <v>13</v>
+      </c>
+      <c r="E3" s="14" t="s">
+        <v>13</v>
+      </c>
+      <c r="F3" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="G3" s="14">
         <v>0.33</v>
       </c>
-      <c r="H3" s="18">
+      <c r="H3" s="14">
         <v>0.79900000000000004</v>
       </c>
-      <c r="I3" s="18">
+      <c r="I3" s="14">
         <v>0.04</v>
       </c>
-      <c r="J3" s="18">
+      <c r="J3" s="14">
         <v>5.6000000000000001E-2</v>
       </c>
-      <c r="K3" s="18">
+      <c r="K3" s="14">
         <v>0.78900000000000003</v>
       </c>
-      <c r="L3" s="18">
+      <c r="L3" s="14">
         <v>0.80900000000000005</v>
       </c>
-      <c r="M3" s="18">
+      <c r="M3" s="14">
         <v>340</v>
       </c>
-      <c r="N3" s="19">
+      <c r="N3" s="15">
         <v>5771</v>
       </c>
     </row>
     <row r="4" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="17">
+      <c r="A4" s="13">
         <v>3</v>
       </c>
-      <c r="B4" s="18" t="s">
+      <c r="B4" s="14" t="s">
         <v>17</v>
       </c>
       <c r="C4" s="2"/>
-      <c r="D4" s="18" t="s">
-        <v>13</v>
-      </c>
-      <c r="E4" s="18" t="s">
-        <v>13</v>
-      </c>
-      <c r="F4" s="18" t="s">
-        <v>14</v>
-      </c>
-      <c r="G4" s="18">
+      <c r="D4" s="14" t="s">
+        <v>13</v>
+      </c>
+      <c r="E4" s="14" t="s">
+        <v>13</v>
+      </c>
+      <c r="F4" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="G4" s="14">
         <v>0.5</v>
       </c>
-      <c r="H4" s="18">
+      <c r="H4" s="14">
         <v>0.80200000000000005</v>
       </c>
-      <c r="I4" s="18">
+      <c r="I4" s="14">
         <v>0.02</v>
       </c>
-      <c r="J4" s="18">
+      <c r="J4" s="14">
         <v>4.9000000000000002E-2</v>
       </c>
-      <c r="K4" s="18">
+      <c r="K4" s="14">
         <v>0.83299999999999996</v>
       </c>
-      <c r="L4" s="18">
+      <c r="L4" s="14">
         <v>0.77200000000000002</v>
       </c>
-      <c r="M4" s="18">
+      <c r="M4" s="14">
         <v>359</v>
       </c>
-      <c r="N4" s="19">
+      <c r="N4" s="15">
         <v>6948</v>
       </c>
     </row>
     <row r="5" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="17">
+      <c r="A5" s="13">
         <v>4</v>
       </c>
-      <c r="B5" s="18" t="s">
+      <c r="B5" s="14" t="s">
         <v>17</v>
       </c>
       <c r="C5" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="D5" s="18" t="s">
-        <v>12</v>
-      </c>
-      <c r="E5" s="18" t="s">
-        <v>13</v>
-      </c>
-      <c r="F5" s="18" t="s">
-        <v>14</v>
-      </c>
-      <c r="G5" s="18">
+      <c r="D5" s="14" t="s">
+        <v>12</v>
+      </c>
+      <c r="E5" s="14" t="s">
+        <v>13</v>
+      </c>
+      <c r="F5" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="G5" s="14">
         <v>0</v>
       </c>
-      <c r="H5" s="18">
+      <c r="H5" s="14">
         <v>0.77100000000000002</v>
       </c>
-      <c r="I5" s="18">
+      <c r="I5" s="14">
         <v>0.2</v>
       </c>
-      <c r="J5" s="18">
+      <c r="J5" s="14">
         <v>4.7E-2</v>
       </c>
-      <c r="K5" s="18">
+      <c r="K5" s="14">
         <v>0.76300000000000001</v>
       </c>
-      <c r="L5" s="18">
+      <c r="L5" s="14">
         <v>0.77800000000000002</v>
       </c>
-      <c r="M5" s="18">
+      <c r="M5" s="14">
         <v>329</v>
       </c>
-      <c r="N5" s="19">
+      <c r="N5" s="15">
         <v>6728</v>
       </c>
     </row>
     <row r="6" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="17">
+      <c r="A6" s="13">
         <v>5</v>
       </c>
-      <c r="B6" s="18" t="s">
+      <c r="B6" s="14" t="s">
         <v>17</v>
       </c>
       <c r="C6" s="2"/>
-      <c r="D6" s="18" t="s">
-        <v>12</v>
-      </c>
-      <c r="E6" s="18" t="s">
-        <v>13</v>
-      </c>
-      <c r="F6" s="18" t="s">
-        <v>14</v>
-      </c>
-      <c r="G6" s="18">
+      <c r="D6" s="14" t="s">
+        <v>12</v>
+      </c>
+      <c r="E6" s="14" t="s">
+        <v>13</v>
+      </c>
+      <c r="F6" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="G6" s="14">
         <v>0.33</v>
       </c>
-      <c r="H6" s="18">
+      <c r="H6" s="14">
         <v>0.80700000000000005</v>
       </c>
-      <c r="I6" s="18">
+      <c r="I6" s="14">
         <v>0.42</v>
       </c>
-      <c r="J6" s="18">
+      <c r="J6" s="14">
         <v>5.5E-2</v>
       </c>
-      <c r="K6" s="18">
+      <c r="K6" s="14">
         <v>0.81399999999999995</v>
       </c>
-      <c r="L6" s="18">
+      <c r="L6" s="14">
         <v>0.8</v>
       </c>
-      <c r="M6" s="18">
+      <c r="M6" s="14">
         <v>351</v>
       </c>
-      <c r="N6" s="19">
+      <c r="N6" s="15">
         <v>6082</v>
       </c>
     </row>
     <row r="7" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="17">
+      <c r="A7" s="13">
         <v>6</v>
       </c>
-      <c r="B7" s="18" t="s">
+      <c r="B7" s="14" t="s">
         <v>17</v>
       </c>
       <c r="C7" s="2"/>
-      <c r="D7" s="18" t="s">
-        <v>12</v>
-      </c>
-      <c r="E7" s="18" t="s">
-        <v>13</v>
-      </c>
-      <c r="F7" s="18" t="s">
-        <v>14</v>
-      </c>
-      <c r="G7" s="18">
+      <c r="D7" s="14" t="s">
+        <v>12</v>
+      </c>
+      <c r="E7" s="14" t="s">
+        <v>13</v>
+      </c>
+      <c r="F7" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="G7" s="14">
         <v>0.5</v>
       </c>
-      <c r="H7" s="18">
+      <c r="H7" s="14">
         <v>0.81100000000000005</v>
       </c>
-      <c r="I7" s="18">
+      <c r="I7" s="14">
         <v>0.43</v>
       </c>
-      <c r="J7" s="18">
+      <c r="J7" s="14">
         <v>5.5E-2</v>
       </c>
-      <c r="K7" s="18">
+      <c r="K7" s="14">
         <v>0.82399999999999995</v>
       </c>
-      <c r="L7" s="18">
+      <c r="L7" s="14">
         <v>0.8</v>
       </c>
-      <c r="M7" s="18">
+      <c r="M7" s="14">
         <v>355</v>
       </c>
-      <c r="N7" s="19">
+      <c r="N7" s="15">
         <v>6089</v>
       </c>
     </row>
     <row r="8" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="17">
+      <c r="A8" s="13">
         <v>7</v>
       </c>
-      <c r="B8" s="18" t="s">
+      <c r="B8" s="14" t="s">
         <v>17</v>
       </c>
       <c r="C8" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="D8" s="18" t="s">
-        <v>12</v>
-      </c>
-      <c r="E8" s="18" t="s">
-        <v>12</v>
-      </c>
-      <c r="F8" s="18" t="s">
+      <c r="D8" s="14" t="s">
+        <v>12</v>
+      </c>
+      <c r="E8" s="14" t="s">
+        <v>12</v>
+      </c>
+      <c r="F8" s="14" t="s">
         <v>15</v>
       </c>
-      <c r="G8" s="18">
+      <c r="G8" s="14">
         <v>0</v>
       </c>
-      <c r="H8" s="18">
+      <c r="H8" s="14">
         <v>0.78700000000000003</v>
       </c>
-      <c r="I8" s="18">
+      <c r="I8" s="14">
         <v>0.19</v>
       </c>
-      <c r="J8" s="18">
+      <c r="J8" s="14">
         <v>5.1999999999999998E-2</v>
       </c>
-      <c r="K8" s="18">
+      <c r="K8" s="14">
         <v>0.77500000000000002</v>
       </c>
-      <c r="L8" s="18">
+      <c r="L8" s="14">
         <v>0.79800000000000004</v>
       </c>
-      <c r="M8" s="18">
+      <c r="M8" s="14">
         <v>334</v>
       </c>
-      <c r="N8" s="19">
+      <c r="N8" s="15">
         <v>6109</v>
       </c>
     </row>
     <row r="9" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="17">
+      <c r="A9" s="13">
         <v>8</v>
       </c>
-      <c r="B9" s="18" t="s">
+      <c r="B9" s="14" t="s">
         <v>17</v>
       </c>
       <c r="C9" s="2"/>
-      <c r="D9" s="18" t="s">
-        <v>12</v>
-      </c>
-      <c r="E9" s="18" t="s">
-        <v>12</v>
-      </c>
-      <c r="F9" s="18" t="s">
+      <c r="D9" s="14" t="s">
+        <v>12</v>
+      </c>
+      <c r="E9" s="14" t="s">
+        <v>12</v>
+      </c>
+      <c r="F9" s="14" t="s">
         <v>15</v>
       </c>
-      <c r="G9" s="18">
+      <c r="G9" s="14">
         <v>0.33</v>
       </c>
-      <c r="H9" s="18">
+      <c r="H9" s="14">
         <v>0.79400000000000004</v>
       </c>
-      <c r="I9" s="18">
+      <c r="I9" s="14">
         <v>0.37</v>
       </c>
-      <c r="J9" s="18">
+      <c r="J9" s="14">
         <v>4.8000000000000001E-2</v>
       </c>
-      <c r="K9" s="18">
+      <c r="K9" s="14">
         <v>0.82099999999999995</v>
       </c>
-      <c r="L9" s="18">
+      <c r="L9" s="14">
         <v>0.76800000000000002</v>
       </c>
-      <c r="M9" s="18">
+      <c r="M9" s="14">
         <v>354</v>
       </c>
-      <c r="N9" s="19">
+      <c r="N9" s="15">
         <v>7050</v>
       </c>
     </row>
     <row r="10" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="17">
+      <c r="A10" s="13">
         <v>9</v>
       </c>
-      <c r="B10" s="18" t="s">
+      <c r="B10" s="14" t="s">
         <v>17</v>
       </c>
       <c r="C10" s="2"/>
-      <c r="D10" s="18" t="s">
-        <v>12</v>
-      </c>
-      <c r="E10" s="18" t="s">
-        <v>12</v>
-      </c>
-      <c r="F10" s="18" t="s">
+      <c r="D10" s="14" t="s">
+        <v>12</v>
+      </c>
+      <c r="E10" s="14" t="s">
+        <v>12</v>
+      </c>
+      <c r="F10" s="14" t="s">
         <v>15</v>
       </c>
-      <c r="G10" s="18">
+      <c r="G10" s="14">
         <v>0.5</v>
       </c>
-      <c r="H10" s="18">
+      <c r="H10" s="14">
         <v>0.80400000000000005</v>
       </c>
-      <c r="I10" s="18">
+      <c r="I10" s="14">
         <v>0.43</v>
       </c>
-      <c r="J10" s="18">
+      <c r="J10" s="14">
         <v>6.0999999999999999E-2</v>
       </c>
-      <c r="K10" s="18">
+      <c r="K10" s="14">
         <v>0.78</v>
       </c>
-      <c r="L10" s="18">
+      <c r="L10" s="14">
         <v>0.82699999999999996</v>
       </c>
-      <c r="M10" s="18">
+      <c r="M10" s="14">
         <v>336</v>
       </c>
-      <c r="N10" s="19">
+      <c r="N10" s="15">
         <v>5211</v>
       </c>
     </row>
     <row r="11" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="17">
+      <c r="A11" s="13">
         <v>10</v>
       </c>
-      <c r="B11" s="18" t="s">
+      <c r="B11" s="14" t="s">
         <v>17</v>
       </c>
       <c r="C11" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="D11" s="18" t="s">
-        <v>12</v>
-      </c>
-      <c r="E11" s="18" t="s">
-        <v>12</v>
-      </c>
-      <c r="F11" s="18" t="s">
+      <c r="D11" s="14" t="s">
+        <v>12</v>
+      </c>
+      <c r="E11" s="14" t="s">
+        <v>12</v>
+      </c>
+      <c r="F11" s="14" t="s">
         <v>16</v>
       </c>
-      <c r="G11" s="18">
+      <c r="G11" s="14">
         <v>0</v>
       </c>
-      <c r="H11" s="18">
+      <c r="H11" s="14">
         <v>0.76600000000000001</v>
       </c>
-      <c r="I11" s="18">
+      <c r="I11" s="14">
         <v>0.03</v>
       </c>
-      <c r="J11" s="18">
+      <c r="J11" s="14">
         <v>4.9000000000000002E-2</v>
       </c>
-      <c r="K11" s="18">
+      <c r="K11" s="14">
         <v>0.73299999999999998</v>
       </c>
-      <c r="L11" s="18">
+      <c r="L11" s="14">
         <v>0.79900000000000004</v>
       </c>
-      <c r="M11" s="18">
+      <c r="M11" s="14">
         <v>316</v>
       </c>
-      <c r="N11" s="19">
+      <c r="N11" s="15">
         <v>6071</v>
       </c>
     </row>
     <row r="12" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="17">
+      <c r="A12" s="13">
         <v>11</v>
       </c>
-      <c r="B12" s="18" t="s">
+      <c r="B12" s="14" t="s">
         <v>17</v>
       </c>
       <c r="C12" s="2"/>
-      <c r="D12" s="18" t="s">
-        <v>12</v>
-      </c>
-      <c r="E12" s="18" t="s">
-        <v>12</v>
-      </c>
-      <c r="F12" s="18" t="s">
+      <c r="D12" s="14" t="s">
+        <v>12</v>
+      </c>
+      <c r="E12" s="14" t="s">
+        <v>12</v>
+      </c>
+      <c r="F12" s="14" t="s">
         <v>16</v>
       </c>
-      <c r="G12" s="18">
+      <c r="G12" s="14">
         <v>0.33</v>
       </c>
-      <c r="H12" s="18">
+      <c r="H12" s="14">
         <v>0.80400000000000005</v>
       </c>
-      <c r="I12" s="18">
+      <c r="I12" s="14">
         <v>0.41</v>
       </c>
-      <c r="J12" s="18">
+      <c r="J12" s="14">
         <v>5.2999999999999999E-2</v>
       </c>
-      <c r="K12" s="18">
+      <c r="K12" s="14">
         <v>0.81699999999999995</v>
       </c>
-      <c r="L12" s="18">
+      <c r="L12" s="14">
         <v>0.79200000000000004</v>
       </c>
-      <c r="M12" s="18">
+      <c r="M12" s="14">
         <v>352</v>
       </c>
-      <c r="N12" s="19">
+      <c r="N12" s="15">
         <v>6310</v>
       </c>
     </row>
     <row r="13" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="17">
-        <v>12</v>
-      </c>
-      <c r="B13" s="18" t="s">
+      <c r="A13" s="13">
+        <v>12</v>
+      </c>
+      <c r="B13" s="14" t="s">
         <v>17</v>
       </c>
       <c r="C13" s="2"/>
-      <c r="D13" s="18" t="s">
-        <v>12</v>
-      </c>
-      <c r="E13" s="18" t="s">
-        <v>12</v>
-      </c>
-      <c r="F13" s="18" t="s">
+      <c r="D13" s="14" t="s">
+        <v>12</v>
+      </c>
+      <c r="E13" s="14" t="s">
+        <v>12</v>
+      </c>
+      <c r="F13" s="14" t="s">
         <v>16</v>
       </c>
-      <c r="G13" s="18">
+      <c r="G13" s="14">
         <v>0.5</v>
       </c>
-      <c r="H13" s="18">
+      <c r="H13" s="14">
         <v>0.80700000000000005</v>
       </c>
-      <c r="I13" s="18">
+      <c r="I13" s="14">
         <v>0.48</v>
       </c>
-      <c r="J13" s="18">
+      <c r="J13" s="14">
         <v>0.06</v>
       </c>
-      <c r="K13" s="18">
+      <c r="K13" s="14">
         <v>0.78900000000000003</v>
       </c>
-      <c r="L13" s="18">
+      <c r="L13" s="14">
         <v>0.82499999999999996</v>
       </c>
-      <c r="M13" s="18">
+      <c r="M13" s="14">
         <v>340</v>
       </c>
-      <c r="N13" s="19">
+      <c r="N13" s="15">
         <v>5298</v>
       </c>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A14" s="14">
+      <c r="A14" s="10">
         <v>13</v>
       </c>
       <c r="B14" s="2" t="s">
@@ -2341,12 +2342,12 @@
       <c r="M14" s="2">
         <v>337</v>
       </c>
-      <c r="N14" s="15">
+      <c r="N14" s="11">
         <v>7231</v>
       </c>
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A15" s="14">
+      <c r="A15" s="10">
         <v>14</v>
       </c>
       <c r="B15" s="2" t="s">
@@ -2383,12 +2384,12 @@
       <c r="M15" s="2">
         <v>339</v>
       </c>
-      <c r="N15" s="15">
+      <c r="N15" s="11">
         <v>7101</v>
       </c>
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A16" s="14">
+      <c r="A16" s="10">
         <v>15</v>
       </c>
       <c r="B16" s="2" t="s">
@@ -2425,15 +2426,15 @@
       <c r="M16" s="2">
         <v>349</v>
       </c>
-      <c r="N16" s="15">
+      <c r="N16" s="11">
         <v>5882</v>
       </c>
     </row>
     <row r="17" spans="1:14" ht="75" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="14">
+      <c r="A17" s="10">
         <v>18</v>
       </c>
-      <c r="B17" s="16" t="s">
+      <c r="B17" s="12" t="s">
         <v>28</v>
       </c>
       <c r="C17" s="2"/>
@@ -2467,126 +2468,126 @@
       <c r="M17" s="2">
         <v>351</v>
       </c>
-      <c r="N17" s="15">
+      <c r="N17" s="11">
         <v>6426</v>
       </c>
     </row>
     <row r="18" spans="1:14" ht="60.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="27">
+      <c r="A18" s="23">
         <v>21</v>
       </c>
-      <c r="B18" s="28" t="s">
+      <c r="B18" s="24" t="s">
         <v>29</v>
       </c>
-      <c r="C18" s="29"/>
-      <c r="D18" s="29" t="s">
-        <v>12</v>
-      </c>
-      <c r="E18" s="29" t="s">
-        <v>13</v>
-      </c>
-      <c r="F18" s="29" t="s">
-        <v>14</v>
-      </c>
-      <c r="G18" s="29">
+      <c r="C18" s="25"/>
+      <c r="D18" s="25" t="s">
+        <v>12</v>
+      </c>
+      <c r="E18" s="25" t="s">
+        <v>13</v>
+      </c>
+      <c r="F18" s="25" t="s">
+        <v>14</v>
+      </c>
+      <c r="G18" s="25">
         <v>0.5</v>
       </c>
-      <c r="H18" s="29">
+      <c r="H18" s="25">
         <v>0.81299999999999994</v>
       </c>
-      <c r="I18" s="29">
+      <c r="I18" s="25">
         <v>0.46</v>
       </c>
-      <c r="J18" s="29">
+      <c r="J18" s="25">
         <v>6.0999999999999999E-2</v>
       </c>
-      <c r="K18" s="29">
+      <c r="K18" s="25">
         <v>0.8</v>
       </c>
-      <c r="L18" s="29">
+      <c r="L18" s="25">
         <v>0.82399999999999995</v>
       </c>
-      <c r="M18" s="29">
+      <c r="M18" s="25">
         <v>345</v>
       </c>
-      <c r="N18" s="30">
+      <c r="N18" s="26">
         <v>5314</v>
       </c>
     </row>
     <row r="19" spans="1:14" ht="20.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="4" t="s">
+      <c r="A19" s="27" t="s">
         <v>20</v>
       </c>
-      <c r="B19" s="5"/>
-      <c r="C19" s="5"/>
-      <c r="D19" s="5"/>
-      <c r="E19" s="5"/>
-      <c r="F19" s="5"/>
-      <c r="G19" s="5"/>
-      <c r="H19" s="6">
+      <c r="B19" s="28"/>
+      <c r="C19" s="28"/>
+      <c r="D19" s="28"/>
+      <c r="E19" s="28"/>
+      <c r="F19" s="28"/>
+      <c r="G19" s="28"/>
+      <c r="H19" s="4">
         <f>AVERAGE(H2:H18)</f>
         <v>0.79517647058823548</v>
       </c>
-      <c r="I19" s="6">
+      <c r="I19" s="4">
         <f t="shared" ref="I19:N19" si="0">AVERAGE(I2:I18)</f>
         <v>0.30352941176470588</v>
       </c>
-      <c r="J19" s="6">
+      <c r="J19" s="4">
         <f t="shared" si="0"/>
         <v>5.2882352941176484E-2</v>
       </c>
-      <c r="K19" s="6">
+      <c r="K19" s="4">
         <f t="shared" si="0"/>
         <v>0.79517647058823537</v>
       </c>
-      <c r="L19" s="6">
+      <c r="L19" s="4">
         <f t="shared" si="0"/>
         <v>0.79170588235294126</v>
       </c>
-      <c r="M19" s="7">
+      <c r="M19" s="5">
         <f t="shared" si="0"/>
         <v>342.70588235294116</v>
       </c>
-      <c r="N19" s="8">
+      <c r="N19" s="6">
         <f t="shared" si="0"/>
         <v>6207.6470588235297</v>
       </c>
     </row>
     <row r="20" spans="1:14" ht="19.5" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="9" t="s">
+      <c r="A20" s="29" t="s">
         <v>21</v>
       </c>
-      <c r="B20" s="10"/>
-      <c r="C20" s="10"/>
-      <c r="D20" s="10"/>
-      <c r="E20" s="10"/>
-      <c r="F20" s="10"/>
-      <c r="G20" s="10"/>
-      <c r="H20" s="11">
+      <c r="B20" s="30"/>
+      <c r="C20" s="30"/>
+      <c r="D20" s="30"/>
+      <c r="E20" s="30"/>
+      <c r="F20" s="30"/>
+      <c r="G20" s="30"/>
+      <c r="H20" s="7">
         <f>_xlfn.STDEV.P(H2:H18)</f>
         <v>1.4697880175756631E-2</v>
       </c>
-      <c r="I20" s="11">
+      <c r="I20" s="7">
         <f t="shared" ref="I20:N20" si="1">_xlfn.STDEV.P(I2:I18)</f>
         <v>0.17931048250157627</v>
       </c>
-      <c r="J20" s="11">
+      <c r="J20" s="7">
         <f t="shared" si="1"/>
         <v>4.9215295678475025E-3</v>
       </c>
-      <c r="K20" s="11">
+      <c r="K20" s="7">
         <f t="shared" si="1"/>
         <v>2.4588938914784763E-2</v>
       </c>
-      <c r="L20" s="11">
+      <c r="L20" s="7">
         <f t="shared" si="1"/>
         <v>2.7970077931882331E-2</v>
       </c>
-      <c r="M20" s="12">
+      <c r="M20" s="8">
         <f t="shared" si="1"/>
         <v>10.598361171217508</v>
       </c>
-      <c r="N20" s="13">
+      <c r="N20" s="9">
         <f t="shared" si="1"/>
         <v>618.13123879456407</v>
       </c>
@@ -2720,563 +2721,563 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" s="1" customFormat="1" ht="44.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="20" t="s">
+      <c r="A1" s="16" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="21" t="s">
+      <c r="B1" s="17" t="s">
         <v>22</v>
       </c>
       <c r="C1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="21" t="s">
+      <c r="D1" s="17" t="s">
         <v>23</v>
       </c>
-      <c r="E1" s="21" t="s">
+      <c r="E1" s="17" t="s">
         <v>24</v>
       </c>
-      <c r="F1" s="21" t="s">
+      <c r="F1" s="17" t="s">
         <v>25</v>
       </c>
-      <c r="G1" s="21" t="s">
+      <c r="G1" s="17" t="s">
         <v>19</v>
       </c>
-      <c r="H1" s="21" t="s">
+      <c r="H1" s="17" t="s">
         <v>18</v>
       </c>
-      <c r="I1" s="21" t="s">
+      <c r="I1" s="17" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="21" t="s">
+      <c r="J1" s="17" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="21" t="s">
+      <c r="K1" s="17" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="21" t="s">
+      <c r="L1" s="17" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="21" t="s">
+      <c r="M1" s="17" t="s">
         <v>26</v>
       </c>
-      <c r="N1" s="22" t="s">
+      <c r="N1" s="18" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="2" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="23">
+      <c r="A2" s="19">
         <v>1</v>
       </c>
-      <c r="B2" s="24" t="s">
-        <v>17</v>
-      </c>
-      <c r="C2" s="25" t="s">
+      <c r="B2" s="20" t="s">
+        <v>17</v>
+      </c>
+      <c r="C2" s="21" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="24" t="s">
-        <v>13</v>
-      </c>
-      <c r="E2" s="24" t="s">
-        <v>13</v>
-      </c>
-      <c r="F2" s="24" t="s">
-        <v>14</v>
-      </c>
-      <c r="G2" s="24">
+      <c r="D2" s="20" t="s">
+        <v>13</v>
+      </c>
+      <c r="E2" s="20" t="s">
+        <v>13</v>
+      </c>
+      <c r="F2" s="20" t="s">
+        <v>14</v>
+      </c>
+      <c r="G2" s="20">
         <v>0</v>
       </c>
-      <c r="H2" s="24">
+      <c r="H2" s="20">
         <v>0.79600000000000004</v>
       </c>
-      <c r="I2" s="24">
+      <c r="I2" s="20">
         <v>0.04</v>
       </c>
-      <c r="J2" s="24">
+      <c r="J2" s="20">
         <v>5.3999999999999999E-2</v>
       </c>
-      <c r="K2" s="24">
+      <c r="K2" s="20">
         <v>0.78700000000000003</v>
       </c>
-      <c r="L2" s="24">
+      <c r="L2" s="20">
         <v>0.80300000000000005</v>
       </c>
-      <c r="M2" s="24">
+      <c r="M2" s="20">
         <v>339</v>
       </c>
-      <c r="N2" s="26">
+      <c r="N2" s="22">
         <v>5909</v>
       </c>
     </row>
     <row r="3" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="17">
+      <c r="A3" s="13">
         <v>2</v>
       </c>
-      <c r="B3" s="18" t="s">
+      <c r="B3" s="14" t="s">
         <v>17</v>
       </c>
       <c r="C3" s="2"/>
-      <c r="D3" s="18" t="s">
-        <v>13</v>
-      </c>
-      <c r="E3" s="18" t="s">
-        <v>13</v>
-      </c>
-      <c r="F3" s="18" t="s">
-        <v>14</v>
-      </c>
-      <c r="G3" s="18">
+      <c r="D3" s="14" t="s">
+        <v>13</v>
+      </c>
+      <c r="E3" s="14" t="s">
+        <v>13</v>
+      </c>
+      <c r="F3" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="G3" s="14">
         <v>0.33</v>
       </c>
-      <c r="H3" s="18">
+      <c r="H3" s="14">
         <v>0.79900000000000004</v>
       </c>
-      <c r="I3" s="18">
+      <c r="I3" s="14">
         <v>0.04</v>
       </c>
-      <c r="J3" s="18">
+      <c r="J3" s="14">
         <v>5.6000000000000001E-2</v>
       </c>
-      <c r="K3" s="18">
+      <c r="K3" s="14">
         <v>0.78900000000000003</v>
       </c>
-      <c r="L3" s="18">
+      <c r="L3" s="14">
         <v>0.80900000000000005</v>
       </c>
-      <c r="M3" s="18">
+      <c r="M3" s="14">
         <v>340</v>
       </c>
-      <c r="N3" s="19">
+      <c r="N3" s="15">
         <v>5771</v>
       </c>
     </row>
     <row r="4" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="17">
+      <c r="A4" s="13">
         <v>3</v>
       </c>
-      <c r="B4" s="18" t="s">
+      <c r="B4" s="14" t="s">
         <v>17</v>
       </c>
       <c r="C4" s="2"/>
-      <c r="D4" s="18" t="s">
-        <v>13</v>
-      </c>
-      <c r="E4" s="18" t="s">
-        <v>13</v>
-      </c>
-      <c r="F4" s="18" t="s">
-        <v>14</v>
-      </c>
-      <c r="G4" s="18">
+      <c r="D4" s="14" t="s">
+        <v>13</v>
+      </c>
+      <c r="E4" s="14" t="s">
+        <v>13</v>
+      </c>
+      <c r="F4" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="G4" s="14">
         <v>0.5</v>
       </c>
-      <c r="H4" s="18">
+      <c r="H4" s="14">
         <v>0.80200000000000005</v>
       </c>
-      <c r="I4" s="18">
+      <c r="I4" s="14">
         <v>0.02</v>
       </c>
-      <c r="J4" s="18">
+      <c r="J4" s="14">
         <v>4.9000000000000002E-2</v>
       </c>
-      <c r="K4" s="18">
+      <c r="K4" s="14">
         <v>0.83299999999999996</v>
       </c>
-      <c r="L4" s="18">
+      <c r="L4" s="14">
         <v>0.77200000000000002</v>
       </c>
-      <c r="M4" s="18">
+      <c r="M4" s="14">
         <v>359</v>
       </c>
-      <c r="N4" s="19">
+      <c r="N4" s="15">
         <v>6948</v>
       </c>
     </row>
     <row r="5" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="17">
+      <c r="A5" s="13">
         <v>4</v>
       </c>
-      <c r="B5" s="18" t="s">
+      <c r="B5" s="14" t="s">
         <v>17</v>
       </c>
       <c r="C5" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="D5" s="18" t="s">
-        <v>12</v>
-      </c>
-      <c r="E5" s="18" t="s">
-        <v>13</v>
-      </c>
-      <c r="F5" s="18" t="s">
-        <v>14</v>
-      </c>
-      <c r="G5" s="18">
+      <c r="D5" s="14" t="s">
+        <v>12</v>
+      </c>
+      <c r="E5" s="14" t="s">
+        <v>13</v>
+      </c>
+      <c r="F5" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="G5" s="14">
         <v>0</v>
       </c>
-      <c r="H5" s="18">
+      <c r="H5" s="14">
         <v>0.77100000000000002</v>
       </c>
-      <c r="I5" s="18">
+      <c r="I5" s="14">
         <v>0.2</v>
       </c>
-      <c r="J5" s="18">
+      <c r="J5" s="14">
         <v>4.7E-2</v>
       </c>
-      <c r="K5" s="18">
+      <c r="K5" s="14">
         <v>0.76300000000000001</v>
       </c>
-      <c r="L5" s="18">
+      <c r="L5" s="14">
         <v>0.77800000000000002</v>
       </c>
-      <c r="M5" s="18">
+      <c r="M5" s="14">
         <v>329</v>
       </c>
-      <c r="N5" s="19">
+      <c r="N5" s="15">
         <v>6728</v>
       </c>
     </row>
     <row r="6" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="17">
+      <c r="A6" s="13">
         <v>5</v>
       </c>
-      <c r="B6" s="18" t="s">
+      <c r="B6" s="14" t="s">
         <v>17</v>
       </c>
       <c r="C6" s="2"/>
-      <c r="D6" s="18" t="s">
-        <v>12</v>
-      </c>
-      <c r="E6" s="18" t="s">
-        <v>13</v>
-      </c>
-      <c r="F6" s="18" t="s">
-        <v>14</v>
-      </c>
-      <c r="G6" s="18">
+      <c r="D6" s="14" t="s">
+        <v>12</v>
+      </c>
+      <c r="E6" s="14" t="s">
+        <v>13</v>
+      </c>
+      <c r="F6" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="G6" s="14">
         <v>0.33</v>
       </c>
-      <c r="H6" s="18">
+      <c r="H6" s="14">
         <v>0.80700000000000005</v>
       </c>
-      <c r="I6" s="18">
+      <c r="I6" s="14">
         <v>0.42</v>
       </c>
-      <c r="J6" s="18">
+      <c r="J6" s="14">
         <v>5.5E-2</v>
       </c>
-      <c r="K6" s="18">
+      <c r="K6" s="14">
         <v>0.81399999999999995</v>
       </c>
-      <c r="L6" s="18">
+      <c r="L6" s="14">
         <v>0.8</v>
       </c>
-      <c r="M6" s="18">
+      <c r="M6" s="14">
         <v>351</v>
       </c>
-      <c r="N6" s="19">
+      <c r="N6" s="15">
         <v>6082</v>
       </c>
     </row>
     <row r="7" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="17">
+      <c r="A7" s="13">
         <v>6</v>
       </c>
-      <c r="B7" s="18" t="s">
+      <c r="B7" s="14" t="s">
         <v>17</v>
       </c>
       <c r="C7" s="2"/>
-      <c r="D7" s="18" t="s">
-        <v>12</v>
-      </c>
-      <c r="E7" s="18" t="s">
-        <v>13</v>
-      </c>
-      <c r="F7" s="18" t="s">
-        <v>14</v>
-      </c>
-      <c r="G7" s="18">
+      <c r="D7" s="14" t="s">
+        <v>12</v>
+      </c>
+      <c r="E7" s="14" t="s">
+        <v>13</v>
+      </c>
+      <c r="F7" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="G7" s="14">
         <v>0.5</v>
       </c>
-      <c r="H7" s="18">
+      <c r="H7" s="14">
         <v>0.81100000000000005</v>
       </c>
-      <c r="I7" s="18">
+      <c r="I7" s="14">
         <v>0.43</v>
       </c>
-      <c r="J7" s="18">
+      <c r="J7" s="14">
         <v>5.5E-2</v>
       </c>
-      <c r="K7" s="18">
+      <c r="K7" s="14">
         <v>0.82399999999999995</v>
       </c>
-      <c r="L7" s="18">
+      <c r="L7" s="14">
         <v>0.8</v>
       </c>
-      <c r="M7" s="18">
+      <c r="M7" s="14">
         <v>355</v>
       </c>
-      <c r="N7" s="19">
+      <c r="N7" s="15">
         <v>6089</v>
       </c>
     </row>
     <row r="8" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="17">
+      <c r="A8" s="13">
         <v>7</v>
       </c>
-      <c r="B8" s="18" t="s">
+      <c r="B8" s="14" t="s">
         <v>17</v>
       </c>
       <c r="C8" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="D8" s="18" t="s">
-        <v>12</v>
-      </c>
-      <c r="E8" s="18" t="s">
-        <v>12</v>
-      </c>
-      <c r="F8" s="18" t="s">
+      <c r="D8" s="14" t="s">
+        <v>12</v>
+      </c>
+      <c r="E8" s="14" t="s">
+        <v>12</v>
+      </c>
+      <c r="F8" s="14" t="s">
         <v>15</v>
       </c>
-      <c r="G8" s="18">
+      <c r="G8" s="14">
         <v>0</v>
       </c>
-      <c r="H8" s="18">
+      <c r="H8" s="14">
         <v>0.78700000000000003</v>
       </c>
-      <c r="I8" s="18">
+      <c r="I8" s="14">
         <v>0.19</v>
       </c>
-      <c r="J8" s="18">
+      <c r="J8" s="14">
         <v>5.1999999999999998E-2</v>
       </c>
-      <c r="K8" s="18">
+      <c r="K8" s="14">
         <v>0.77500000000000002</v>
       </c>
-      <c r="L8" s="18">
+      <c r="L8" s="14">
         <v>0.79800000000000004</v>
       </c>
-      <c r="M8" s="18">
+      <c r="M8" s="14">
         <v>334</v>
       </c>
-      <c r="N8" s="19">
+      <c r="N8" s="15">
         <v>6109</v>
       </c>
     </row>
     <row r="9" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="17">
+      <c r="A9" s="13">
         <v>8</v>
       </c>
-      <c r="B9" s="18" t="s">
+      <c r="B9" s="14" t="s">
         <v>17</v>
       </c>
       <c r="C9" s="2"/>
-      <c r="D9" s="18" t="s">
-        <v>12</v>
-      </c>
-      <c r="E9" s="18" t="s">
-        <v>12</v>
-      </c>
-      <c r="F9" s="18" t="s">
+      <c r="D9" s="14" t="s">
+        <v>12</v>
+      </c>
+      <c r="E9" s="14" t="s">
+        <v>12</v>
+      </c>
+      <c r="F9" s="14" t="s">
         <v>15</v>
       </c>
-      <c r="G9" s="18">
+      <c r="G9" s="14">
         <v>0.33</v>
       </c>
-      <c r="H9" s="18">
+      <c r="H9" s="14">
         <v>0.79400000000000004</v>
       </c>
-      <c r="I9" s="18">
+      <c r="I9" s="14">
         <v>0.37</v>
       </c>
-      <c r="J9" s="18">
+      <c r="J9" s="14">
         <v>4.8000000000000001E-2</v>
       </c>
-      <c r="K9" s="18">
+      <c r="K9" s="14">
         <v>0.82099999999999995</v>
       </c>
-      <c r="L9" s="18">
+      <c r="L9" s="14">
         <v>0.76800000000000002</v>
       </c>
-      <c r="M9" s="18">
+      <c r="M9" s="14">
         <v>354</v>
       </c>
-      <c r="N9" s="19">
+      <c r="N9" s="15">
         <v>7050</v>
       </c>
     </row>
     <row r="10" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="17">
+      <c r="A10" s="13">
         <v>9</v>
       </c>
-      <c r="B10" s="18" t="s">
+      <c r="B10" s="14" t="s">
         <v>17</v>
       </c>
       <c r="C10" s="2"/>
-      <c r="D10" s="18" t="s">
-        <v>12</v>
-      </c>
-      <c r="E10" s="18" t="s">
-        <v>12</v>
-      </c>
-      <c r="F10" s="18" t="s">
+      <c r="D10" s="14" t="s">
+        <v>12</v>
+      </c>
+      <c r="E10" s="14" t="s">
+        <v>12</v>
+      </c>
+      <c r="F10" s="14" t="s">
         <v>15</v>
       </c>
-      <c r="G10" s="18">
+      <c r="G10" s="14">
         <v>0.5</v>
       </c>
-      <c r="H10" s="18">
+      <c r="H10" s="14">
         <v>0.80400000000000005</v>
       </c>
-      <c r="I10" s="18">
+      <c r="I10" s="14">
         <v>0.43</v>
       </c>
-      <c r="J10" s="18">
+      <c r="J10" s="14">
         <v>6.0999999999999999E-2</v>
       </c>
-      <c r="K10" s="18">
+      <c r="K10" s="14">
         <v>0.78</v>
       </c>
-      <c r="L10" s="18">
+      <c r="L10" s="14">
         <v>0.82699999999999996</v>
       </c>
-      <c r="M10" s="18">
+      <c r="M10" s="14">
         <v>336</v>
       </c>
-      <c r="N10" s="19">
+      <c r="N10" s="15">
         <v>5211</v>
       </c>
     </row>
     <row r="11" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="17">
+      <c r="A11" s="13">
         <v>10</v>
       </c>
-      <c r="B11" s="18" t="s">
+      <c r="B11" s="14" t="s">
         <v>17</v>
       </c>
       <c r="C11" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="D11" s="18" t="s">
-        <v>12</v>
-      </c>
-      <c r="E11" s="18" t="s">
-        <v>12</v>
-      </c>
-      <c r="F11" s="18" t="s">
+      <c r="D11" s="14" t="s">
+        <v>12</v>
+      </c>
+      <c r="E11" s="14" t="s">
+        <v>12</v>
+      </c>
+      <c r="F11" s="14" t="s">
         <v>16</v>
       </c>
-      <c r="G11" s="18">
+      <c r="G11" s="14">
         <v>0</v>
       </c>
-      <c r="H11" s="18">
+      <c r="H11" s="14">
         <v>0.76600000000000001</v>
       </c>
-      <c r="I11" s="18">
+      <c r="I11" s="14">
         <v>0.03</v>
       </c>
-      <c r="J11" s="18">
+      <c r="J11" s="14">
         <v>4.9000000000000002E-2</v>
       </c>
-      <c r="K11" s="18">
+      <c r="K11" s="14">
         <v>0.73299999999999998</v>
       </c>
-      <c r="L11" s="18">
+      <c r="L11" s="14">
         <v>0.79900000000000004</v>
       </c>
-      <c r="M11" s="18">
+      <c r="M11" s="14">
         <v>316</v>
       </c>
-      <c r="N11" s="19">
+      <c r="N11" s="15">
         <v>6071</v>
       </c>
     </row>
     <row r="12" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="17">
+      <c r="A12" s="13">
         <v>11</v>
       </c>
-      <c r="B12" s="18" t="s">
+      <c r="B12" s="14" t="s">
         <v>17</v>
       </c>
       <c r="C12" s="2"/>
-      <c r="D12" s="18" t="s">
-        <v>12</v>
-      </c>
-      <c r="E12" s="18" t="s">
-        <v>12</v>
-      </c>
-      <c r="F12" s="18" t="s">
+      <c r="D12" s="14" t="s">
+        <v>12</v>
+      </c>
+      <c r="E12" s="14" t="s">
+        <v>12</v>
+      </c>
+      <c r="F12" s="14" t="s">
         <v>16</v>
       </c>
-      <c r="G12" s="18">
+      <c r="G12" s="14">
         <v>0.33</v>
       </c>
-      <c r="H12" s="18">
+      <c r="H12" s="14">
         <v>0.80400000000000005</v>
       </c>
-      <c r="I12" s="18">
+      <c r="I12" s="14">
         <v>0.41</v>
       </c>
-      <c r="J12" s="18">
+      <c r="J12" s="14">
         <v>5.2999999999999999E-2</v>
       </c>
-      <c r="K12" s="18">
+      <c r="K12" s="14">
         <v>0.81699999999999995</v>
       </c>
-      <c r="L12" s="18">
+      <c r="L12" s="14">
         <v>0.79200000000000004</v>
       </c>
-      <c r="M12" s="18">
+      <c r="M12" s="14">
         <v>352</v>
       </c>
-      <c r="N12" s="19">
+      <c r="N12" s="15">
         <v>6310</v>
       </c>
     </row>
     <row r="13" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="17">
-        <v>12</v>
-      </c>
-      <c r="B13" s="18" t="s">
+      <c r="A13" s="13">
+        <v>12</v>
+      </c>
+      <c r="B13" s="14" t="s">
         <v>17</v>
       </c>
       <c r="C13" s="2"/>
-      <c r="D13" s="18" t="s">
-        <v>12</v>
-      </c>
-      <c r="E13" s="18" t="s">
-        <v>12</v>
-      </c>
-      <c r="F13" s="18" t="s">
+      <c r="D13" s="14" t="s">
+        <v>12</v>
+      </c>
+      <c r="E13" s="14" t="s">
+        <v>12</v>
+      </c>
+      <c r="F13" s="14" t="s">
         <v>16</v>
       </c>
-      <c r="G13" s="18">
+      <c r="G13" s="14">
         <v>0.5</v>
       </c>
-      <c r="H13" s="18">
+      <c r="H13" s="14">
         <v>0.80700000000000005</v>
       </c>
-      <c r="I13" s="18">
+      <c r="I13" s="14">
         <v>0.48</v>
       </c>
-      <c r="J13" s="18">
+      <c r="J13" s="14">
         <v>0.06</v>
       </c>
-      <c r="K13" s="18">
+      <c r="K13" s="14">
         <v>0.78900000000000003</v>
       </c>
-      <c r="L13" s="18">
+      <c r="L13" s="14">
         <v>0.82499999999999996</v>
       </c>
-      <c r="M13" s="18">
+      <c r="M13" s="14">
         <v>340</v>
       </c>
-      <c r="N13" s="19">
+      <c r="N13" s="15">
         <v>5298</v>
       </c>
     </row>
     <row r="14" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="14">
+      <c r="A14" s="10">
         <v>13</v>
       </c>
       <c r="B14" s="2" t="s">
@@ -3315,12 +3316,12 @@
       <c r="M14" s="2">
         <v>337</v>
       </c>
-      <c r="N14" s="15">
+      <c r="N14" s="11">
         <v>7231</v>
       </c>
     </row>
     <row r="15" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="14">
+      <c r="A15" s="10">
         <v>14</v>
       </c>
       <c r="B15" s="2" t="s">
@@ -3357,12 +3358,12 @@
       <c r="M15" s="2">
         <v>339</v>
       </c>
-      <c r="N15" s="15">
+      <c r="N15" s="11">
         <v>7101</v>
       </c>
     </row>
     <row r="16" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="14">
+      <c r="A16" s="10">
         <v>15</v>
       </c>
       <c r="B16" s="2" t="s">
@@ -3399,15 +3400,15 @@
       <c r="M16" s="2">
         <v>349</v>
       </c>
-      <c r="N16" s="15">
+      <c r="N16" s="11">
         <v>5882</v>
       </c>
     </row>
     <row r="17" spans="1:14" ht="75" x14ac:dyDescent="0.25">
-      <c r="A17" s="14">
+      <c r="A17" s="10">
         <v>18</v>
       </c>
-      <c r="B17" s="16" t="s">
+      <c r="B17" s="12" t="s">
         <v>28</v>
       </c>
       <c r="C17" s="2"/>
@@ -3441,126 +3442,126 @@
       <c r="M17" s="2">
         <v>351</v>
       </c>
-      <c r="N17" s="15">
+      <c r="N17" s="11">
         <v>6426</v>
       </c>
     </row>
     <row r="18" spans="1:14" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="27">
+      <c r="A18" s="23">
         <v>21</v>
       </c>
-      <c r="B18" s="28" t="s">
+      <c r="B18" s="24" t="s">
         <v>29</v>
       </c>
-      <c r="C18" s="29"/>
-      <c r="D18" s="29" t="s">
-        <v>12</v>
-      </c>
-      <c r="E18" s="29" t="s">
-        <v>13</v>
-      </c>
-      <c r="F18" s="29" t="s">
-        <v>14</v>
-      </c>
-      <c r="G18" s="29">
+      <c r="C18" s="25"/>
+      <c r="D18" s="25" t="s">
+        <v>12</v>
+      </c>
+      <c r="E18" s="25" t="s">
+        <v>13</v>
+      </c>
+      <c r="F18" s="25" t="s">
+        <v>14</v>
+      </c>
+      <c r="G18" s="25">
         <v>0.5</v>
       </c>
-      <c r="H18" s="29">
+      <c r="H18" s="25">
         <v>0.81299999999999994</v>
       </c>
-      <c r="I18" s="29">
+      <c r="I18" s="25">
         <v>0.46</v>
       </c>
-      <c r="J18" s="29">
+      <c r="J18" s="25">
         <v>6.0999999999999999E-2</v>
       </c>
-      <c r="K18" s="29">
+      <c r="K18" s="25">
         <v>0.8</v>
       </c>
-      <c r="L18" s="29">
+      <c r="L18" s="25">
         <v>0.82399999999999995</v>
       </c>
-      <c r="M18" s="29">
+      <c r="M18" s="25">
         <v>345</v>
       </c>
-      <c r="N18" s="30">
+      <c r="N18" s="26">
         <v>5314</v>
       </c>
     </row>
     <row r="19" spans="1:14" ht="20.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="4" t="s">
+      <c r="A19" s="27" t="s">
         <v>20</v>
       </c>
-      <c r="B19" s="5"/>
-      <c r="C19" s="5"/>
-      <c r="D19" s="5"/>
-      <c r="E19" s="5"/>
-      <c r="F19" s="5"/>
-      <c r="G19" s="5"/>
-      <c r="H19" s="6">
+      <c r="B19" s="28"/>
+      <c r="C19" s="28"/>
+      <c r="D19" s="28"/>
+      <c r="E19" s="28"/>
+      <c r="F19" s="28"/>
+      <c r="G19" s="28"/>
+      <c r="H19" s="4">
         <f>AVERAGE(H2:H18)</f>
         <v>0.79517647058823548</v>
       </c>
-      <c r="I19" s="6">
+      <c r="I19" s="4">
         <f t="shared" ref="I19:N19" si="0">AVERAGE(I2:I18)</f>
         <v>0.30352941176470588</v>
       </c>
-      <c r="J19" s="6">
+      <c r="J19" s="4">
         <f t="shared" si="0"/>
         <v>5.2882352941176484E-2</v>
       </c>
-      <c r="K19" s="6">
+      <c r="K19" s="4">
         <f t="shared" si="0"/>
         <v>0.79517647058823537</v>
       </c>
-      <c r="L19" s="6">
+      <c r="L19" s="4">
         <f t="shared" si="0"/>
         <v>0.79170588235294126</v>
       </c>
-      <c r="M19" s="7">
+      <c r="M19" s="5">
         <f t="shared" si="0"/>
         <v>342.70588235294116</v>
       </c>
-      <c r="N19" s="8">
+      <c r="N19" s="6">
         <f t="shared" si="0"/>
         <v>6207.6470588235297</v>
       </c>
     </row>
     <row r="20" spans="1:14" ht="19.5" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="9" t="s">
+      <c r="A20" s="29" t="s">
         <v>21</v>
       </c>
-      <c r="B20" s="10"/>
-      <c r="C20" s="10"/>
-      <c r="D20" s="10"/>
-      <c r="E20" s="10"/>
-      <c r="F20" s="10"/>
-      <c r="G20" s="10"/>
-      <c r="H20" s="11">
+      <c r="B20" s="30"/>
+      <c r="C20" s="30"/>
+      <c r="D20" s="30"/>
+      <c r="E20" s="30"/>
+      <c r="F20" s="30"/>
+      <c r="G20" s="30"/>
+      <c r="H20" s="7">
         <f>_xlfn.STDEV.P(H2:H18)</f>
         <v>1.4697880175756631E-2</v>
       </c>
-      <c r="I20" s="11">
+      <c r="I20" s="7">
         <f t="shared" ref="I20:N20" si="1">_xlfn.STDEV.P(I2:I18)</f>
         <v>0.17931048250157627</v>
       </c>
-      <c r="J20" s="11">
+      <c r="J20" s="7">
         <f t="shared" si="1"/>
         <v>4.9215295678475025E-3</v>
       </c>
-      <c r="K20" s="11">
+      <c r="K20" s="7">
         <f t="shared" si="1"/>
         <v>2.4588938914784763E-2</v>
       </c>
-      <c r="L20" s="11">
+      <c r="L20" s="7">
         <f t="shared" si="1"/>
         <v>2.7970077931882331E-2</v>
       </c>
-      <c r="M20" s="12">
+      <c r="M20" s="8">
         <f t="shared" si="1"/>
         <v>10.598361171217508</v>
       </c>
-      <c r="N20" s="13">
+      <c r="N20" s="9">
         <f t="shared" si="1"/>
         <v>618.13123879456407</v>
       </c>
@@ -3671,8 +3672,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2C7E5601-8D6A-455E-9FE6-05ADB055289C}">
   <dimension ref="A1:N20"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
-      <selection activeCell="P14" sqref="P14"/>
+    <sheetView tabSelected="1" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
+      <selection activeCell="P8" sqref="P8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3694,563 +3695,563 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" s="1" customFormat="1" ht="44.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="20" t="s">
+      <c r="A1" s="16" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="21" t="s">
+      <c r="B1" s="17" t="s">
         <v>22</v>
       </c>
       <c r="C1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="21" t="s">
+      <c r="D1" s="17" t="s">
         <v>23</v>
       </c>
-      <c r="E1" s="21" t="s">
+      <c r="E1" s="17" t="s">
         <v>24</v>
       </c>
-      <c r="F1" s="21" t="s">
+      <c r="F1" s="17" t="s">
         <v>25</v>
       </c>
-      <c r="G1" s="21" t="s">
+      <c r="G1" s="17" t="s">
         <v>19</v>
       </c>
-      <c r="H1" s="21" t="s">
+      <c r="H1" s="17" t="s">
         <v>18</v>
       </c>
-      <c r="I1" s="21" t="s">
+      <c r="I1" s="17" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="21" t="s">
+      <c r="J1" s="17" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="21" t="s">
+      <c r="K1" s="17" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="21" t="s">
+      <c r="L1" s="17" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="21" t="s">
+      <c r="M1" s="17" t="s">
         <v>26</v>
       </c>
-      <c r="N1" s="22" t="s">
+      <c r="N1" s="18" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A2" s="23">
+      <c r="A2" s="19">
         <v>1</v>
       </c>
-      <c r="B2" s="24" t="s">
-        <v>17</v>
-      </c>
-      <c r="C2" s="25" t="s">
+      <c r="B2" s="20" t="s">
+        <v>17</v>
+      </c>
+      <c r="C2" s="21" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="24" t="s">
-        <v>13</v>
-      </c>
-      <c r="E2" s="24" t="s">
-        <v>13</v>
-      </c>
-      <c r="F2" s="24" t="s">
-        <v>14</v>
-      </c>
-      <c r="G2" s="24">
+      <c r="D2" s="20" t="s">
+        <v>13</v>
+      </c>
+      <c r="E2" s="20" t="s">
+        <v>13</v>
+      </c>
+      <c r="F2" s="20" t="s">
+        <v>14</v>
+      </c>
+      <c r="G2" s="20">
         <v>0</v>
       </c>
-      <c r="H2" s="24">
+      <c r="H2" s="20">
         <v>0.79600000000000004</v>
       </c>
-      <c r="I2" s="24">
+      <c r="I2" s="20">
         <v>0.04</v>
       </c>
-      <c r="J2" s="24">
+      <c r="J2" s="20">
         <v>5.3999999999999999E-2</v>
       </c>
-      <c r="K2" s="24">
+      <c r="K2" s="20">
         <v>0.78700000000000003</v>
       </c>
-      <c r="L2" s="24">
+      <c r="L2" s="20">
         <v>0.80300000000000005</v>
       </c>
-      <c r="M2" s="24">
+      <c r="M2" s="20">
         <v>339</v>
       </c>
-      <c r="N2" s="26">
+      <c r="N2" s="22">
         <v>5909</v>
       </c>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A3" s="17">
+      <c r="A3" s="13">
         <v>2</v>
       </c>
-      <c r="B3" s="18" t="s">
+      <c r="B3" s="14" t="s">
         <v>17</v>
       </c>
       <c r="C3" s="2"/>
-      <c r="D3" s="18" t="s">
-        <v>13</v>
-      </c>
-      <c r="E3" s="18" t="s">
-        <v>13</v>
-      </c>
-      <c r="F3" s="18" t="s">
-        <v>14</v>
-      </c>
-      <c r="G3" s="18">
+      <c r="D3" s="14" t="s">
+        <v>13</v>
+      </c>
+      <c r="E3" s="14" t="s">
+        <v>13</v>
+      </c>
+      <c r="F3" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="G3" s="14">
         <v>0.33</v>
       </c>
-      <c r="H3" s="18">
+      <c r="H3" s="14">
         <v>0.79900000000000004</v>
       </c>
-      <c r="I3" s="18">
+      <c r="I3" s="14">
         <v>0.04</v>
       </c>
-      <c r="J3" s="18">
+      <c r="J3" s="14">
         <v>5.6000000000000001E-2</v>
       </c>
-      <c r="K3" s="18">
+      <c r="K3" s="14">
         <v>0.78900000000000003</v>
       </c>
-      <c r="L3" s="18">
+      <c r="L3" s="14">
         <v>0.80900000000000005</v>
       </c>
-      <c r="M3" s="18">
+      <c r="M3" s="14">
         <v>340</v>
       </c>
-      <c r="N3" s="19">
+      <c r="N3" s="15">
         <v>5771</v>
       </c>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A4" s="17">
+      <c r="A4" s="13">
         <v>3</v>
       </c>
-      <c r="B4" s="18" t="s">
+      <c r="B4" s="14" t="s">
         <v>17</v>
       </c>
       <c r="C4" s="2"/>
-      <c r="D4" s="18" t="s">
-        <v>13</v>
-      </c>
-      <c r="E4" s="18" t="s">
-        <v>13</v>
-      </c>
-      <c r="F4" s="18" t="s">
-        <v>14</v>
-      </c>
-      <c r="G4" s="18">
+      <c r="D4" s="14" t="s">
+        <v>13</v>
+      </c>
+      <c r="E4" s="14" t="s">
+        <v>13</v>
+      </c>
+      <c r="F4" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="G4" s="14">
         <v>0.5</v>
       </c>
-      <c r="H4" s="18">
+      <c r="H4" s="14">
         <v>0.80200000000000005</v>
       </c>
-      <c r="I4" s="18">
+      <c r="I4" s="14">
         <v>0.02</v>
       </c>
-      <c r="J4" s="18">
+      <c r="J4" s="14">
         <v>4.9000000000000002E-2</v>
       </c>
-      <c r="K4" s="18">
+      <c r="K4" s="14">
         <v>0.83299999999999996</v>
       </c>
-      <c r="L4" s="18">
+      <c r="L4" s="14">
         <v>0.77200000000000002</v>
       </c>
-      <c r="M4" s="18">
+      <c r="M4" s="14">
         <v>359</v>
       </c>
-      <c r="N4" s="19">
+      <c r="N4" s="15">
         <v>6948</v>
       </c>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A5" s="17">
+      <c r="A5" s="13">
         <v>4</v>
       </c>
-      <c r="B5" s="18" t="s">
+      <c r="B5" s="14" t="s">
         <v>17</v>
       </c>
       <c r="C5" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="D5" s="18" t="s">
-        <v>12</v>
-      </c>
-      <c r="E5" s="18" t="s">
-        <v>13</v>
-      </c>
-      <c r="F5" s="18" t="s">
-        <v>14</v>
-      </c>
-      <c r="G5" s="18">
+      <c r="D5" s="14" t="s">
+        <v>12</v>
+      </c>
+      <c r="E5" s="14" t="s">
+        <v>13</v>
+      </c>
+      <c r="F5" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="G5" s="14">
         <v>0</v>
       </c>
-      <c r="H5" s="18">
+      <c r="H5" s="14">
         <v>0.77100000000000002</v>
       </c>
-      <c r="I5" s="18">
+      <c r="I5" s="14">
         <v>0.2</v>
       </c>
-      <c r="J5" s="18">
+      <c r="J5" s="14">
         <v>4.7E-2</v>
       </c>
-      <c r="K5" s="18">
+      <c r="K5" s="14">
         <v>0.76300000000000001</v>
       </c>
-      <c r="L5" s="18">
+      <c r="L5" s="14">
         <v>0.77800000000000002</v>
       </c>
-      <c r="M5" s="18">
+      <c r="M5" s="14">
         <v>329</v>
       </c>
-      <c r="N5" s="19">
+      <c r="N5" s="15">
         <v>6728</v>
       </c>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A6" s="17">
+      <c r="A6" s="13">
         <v>5</v>
       </c>
-      <c r="B6" s="18" t="s">
+      <c r="B6" s="14" t="s">
         <v>17</v>
       </c>
       <c r="C6" s="2"/>
-      <c r="D6" s="18" t="s">
-        <v>12</v>
-      </c>
-      <c r="E6" s="18" t="s">
-        <v>13</v>
-      </c>
-      <c r="F6" s="18" t="s">
-        <v>14</v>
-      </c>
-      <c r="G6" s="18">
+      <c r="D6" s="14" t="s">
+        <v>12</v>
+      </c>
+      <c r="E6" s="14" t="s">
+        <v>13</v>
+      </c>
+      <c r="F6" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="G6" s="14">
         <v>0.33</v>
       </c>
-      <c r="H6" s="18">
+      <c r="H6" s="14">
         <v>0.80700000000000005</v>
       </c>
-      <c r="I6" s="18">
+      <c r="I6" s="14">
         <v>0.42</v>
       </c>
-      <c r="J6" s="18">
+      <c r="J6" s="14">
         <v>5.5E-2</v>
       </c>
-      <c r="K6" s="18">
+      <c r="K6" s="14">
         <v>0.81399999999999995</v>
       </c>
-      <c r="L6" s="18">
+      <c r="L6" s="14">
         <v>0.8</v>
       </c>
-      <c r="M6" s="18">
+      <c r="M6" s="14">
         <v>351</v>
       </c>
-      <c r="N6" s="19">
+      <c r="N6" s="15">
         <v>6082</v>
       </c>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A7" s="17">
+      <c r="A7" s="13">
         <v>6</v>
       </c>
-      <c r="B7" s="18" t="s">
+      <c r="B7" s="14" t="s">
         <v>17</v>
       </c>
       <c r="C7" s="2"/>
-      <c r="D7" s="18" t="s">
-        <v>12</v>
-      </c>
-      <c r="E7" s="18" t="s">
-        <v>13</v>
-      </c>
-      <c r="F7" s="18" t="s">
-        <v>14</v>
-      </c>
-      <c r="G7" s="18">
+      <c r="D7" s="14" t="s">
+        <v>12</v>
+      </c>
+      <c r="E7" s="14" t="s">
+        <v>13</v>
+      </c>
+      <c r="F7" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="G7" s="14">
         <v>0.5</v>
       </c>
-      <c r="H7" s="18">
+      <c r="H7" s="14">
         <v>0.81100000000000005</v>
       </c>
-      <c r="I7" s="18">
+      <c r="I7" s="14">
         <v>0.43</v>
       </c>
-      <c r="J7" s="18">
+      <c r="J7" s="14">
         <v>5.5E-2</v>
       </c>
-      <c r="K7" s="18">
+      <c r="K7" s="14">
         <v>0.82399999999999995</v>
       </c>
-      <c r="L7" s="18">
+      <c r="L7" s="14">
         <v>0.8</v>
       </c>
-      <c r="M7" s="18">
+      <c r="M7" s="14">
         <v>355</v>
       </c>
-      <c r="N7" s="19">
+      <c r="N7" s="15">
         <v>6089</v>
       </c>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A8" s="17">
+      <c r="A8" s="13">
         <v>7</v>
       </c>
-      <c r="B8" s="18" t="s">
+      <c r="B8" s="14" t="s">
         <v>17</v>
       </c>
       <c r="C8" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="D8" s="18" t="s">
-        <v>12</v>
-      </c>
-      <c r="E8" s="18" t="s">
-        <v>12</v>
-      </c>
-      <c r="F8" s="18" t="s">
+      <c r="D8" s="14" t="s">
+        <v>12</v>
+      </c>
+      <c r="E8" s="14" t="s">
+        <v>12</v>
+      </c>
+      <c r="F8" s="14" t="s">
         <v>15</v>
       </c>
-      <c r="G8" s="18">
+      <c r="G8" s="14">
         <v>0</v>
       </c>
-      <c r="H8" s="18">
+      <c r="H8" s="14">
         <v>0.78700000000000003</v>
       </c>
-      <c r="I8" s="18">
+      <c r="I8" s="14">
         <v>0.19</v>
       </c>
-      <c r="J8" s="18">
+      <c r="J8" s="14">
         <v>5.1999999999999998E-2</v>
       </c>
-      <c r="K8" s="18">
+      <c r="K8" s="14">
         <v>0.77500000000000002</v>
       </c>
-      <c r="L8" s="18">
+      <c r="L8" s="14">
         <v>0.79800000000000004</v>
       </c>
-      <c r="M8" s="18">
+      <c r="M8" s="14">
         <v>334</v>
       </c>
-      <c r="N8" s="19">
+      <c r="N8" s="15">
         <v>6109</v>
       </c>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A9" s="17">
+      <c r="A9" s="13">
         <v>8</v>
       </c>
-      <c r="B9" s="18" t="s">
+      <c r="B9" s="14" t="s">
         <v>17</v>
       </c>
       <c r="C9" s="2"/>
-      <c r="D9" s="18" t="s">
-        <v>12</v>
-      </c>
-      <c r="E9" s="18" t="s">
-        <v>12</v>
-      </c>
-      <c r="F9" s="18" t="s">
+      <c r="D9" s="14" t="s">
+        <v>12</v>
+      </c>
+      <c r="E9" s="14" t="s">
+        <v>12</v>
+      </c>
+      <c r="F9" s="14" t="s">
         <v>15</v>
       </c>
-      <c r="G9" s="18">
+      <c r="G9" s="14">
         <v>0.33</v>
       </c>
-      <c r="H9" s="18">
+      <c r="H9" s="14">
         <v>0.79400000000000004</v>
       </c>
-      <c r="I9" s="18">
+      <c r="I9" s="14">
         <v>0.37</v>
       </c>
-      <c r="J9" s="18">
+      <c r="J9" s="14">
         <v>4.8000000000000001E-2</v>
       </c>
-      <c r="K9" s="18">
+      <c r="K9" s="14">
         <v>0.82099999999999995</v>
       </c>
-      <c r="L9" s="18">
+      <c r="L9" s="14">
         <v>0.76800000000000002</v>
       </c>
-      <c r="M9" s="18">
+      <c r="M9" s="14">
         <v>354</v>
       </c>
-      <c r="N9" s="19">
+      <c r="N9" s="15">
         <v>7050</v>
       </c>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A10" s="17">
+      <c r="A10" s="13">
         <v>9</v>
       </c>
-      <c r="B10" s="18" t="s">
+      <c r="B10" s="14" t="s">
         <v>17</v>
       </c>
       <c r="C10" s="2"/>
-      <c r="D10" s="18" t="s">
-        <v>12</v>
-      </c>
-      <c r="E10" s="18" t="s">
-        <v>12</v>
-      </c>
-      <c r="F10" s="18" t="s">
+      <c r="D10" s="14" t="s">
+        <v>12</v>
+      </c>
+      <c r="E10" s="14" t="s">
+        <v>12</v>
+      </c>
+      <c r="F10" s="14" t="s">
         <v>15</v>
       </c>
-      <c r="G10" s="18">
+      <c r="G10" s="14">
         <v>0.5</v>
       </c>
-      <c r="H10" s="18">
+      <c r="H10" s="14">
         <v>0.80400000000000005</v>
       </c>
-      <c r="I10" s="18">
+      <c r="I10" s="14">
         <v>0.43</v>
       </c>
-      <c r="J10" s="18">
+      <c r="J10" s="14">
         <v>6.0999999999999999E-2</v>
       </c>
-      <c r="K10" s="18">
+      <c r="K10" s="14">
         <v>0.78</v>
       </c>
-      <c r="L10" s="18">
+      <c r="L10" s="14">
         <v>0.82699999999999996</v>
       </c>
-      <c r="M10" s="18">
+      <c r="M10" s="14">
         <v>336</v>
       </c>
-      <c r="N10" s="19">
+      <c r="N10" s="15">
         <v>5211</v>
       </c>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A11" s="17">
+      <c r="A11" s="13">
         <v>10</v>
       </c>
-      <c r="B11" s="18" t="s">
+      <c r="B11" s="14" t="s">
         <v>17</v>
       </c>
       <c r="C11" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="D11" s="18" t="s">
-        <v>12</v>
-      </c>
-      <c r="E11" s="18" t="s">
-        <v>12</v>
-      </c>
-      <c r="F11" s="18" t="s">
+      <c r="D11" s="14" t="s">
+        <v>12</v>
+      </c>
+      <c r="E11" s="14" t="s">
+        <v>12</v>
+      </c>
+      <c r="F11" s="14" t="s">
         <v>16</v>
       </c>
-      <c r="G11" s="18">
+      <c r="G11" s="14">
         <v>0</v>
       </c>
-      <c r="H11" s="18">
+      <c r="H11" s="14">
         <v>0.76600000000000001</v>
       </c>
-      <c r="I11" s="18">
+      <c r="I11" s="14">
         <v>0.03</v>
       </c>
-      <c r="J11" s="18">
+      <c r="J11" s="14">
         <v>4.9000000000000002E-2</v>
       </c>
-      <c r="K11" s="18">
+      <c r="K11" s="14">
         <v>0.73299999999999998</v>
       </c>
-      <c r="L11" s="18">
+      <c r="L11" s="14">
         <v>0.79900000000000004</v>
       </c>
-      <c r="M11" s="18">
+      <c r="M11" s="14">
         <v>316</v>
       </c>
-      <c r="N11" s="19">
+      <c r="N11" s="15">
         <v>6071</v>
       </c>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A12" s="17">
+      <c r="A12" s="13">
         <v>11</v>
       </c>
-      <c r="B12" s="18" t="s">
+      <c r="B12" s="14" t="s">
         <v>17</v>
       </c>
       <c r="C12" s="2"/>
-      <c r="D12" s="18" t="s">
-        <v>12</v>
-      </c>
-      <c r="E12" s="18" t="s">
-        <v>12</v>
-      </c>
-      <c r="F12" s="18" t="s">
+      <c r="D12" s="14" t="s">
+        <v>12</v>
+      </c>
+      <c r="E12" s="14" t="s">
+        <v>12</v>
+      </c>
+      <c r="F12" s="14" t="s">
         <v>16</v>
       </c>
-      <c r="G12" s="18">
+      <c r="G12" s="14">
         <v>0.33</v>
       </c>
-      <c r="H12" s="18">
+      <c r="H12" s="14">
         <v>0.80400000000000005</v>
       </c>
-      <c r="I12" s="18">
+      <c r="I12" s="14">
         <v>0.41</v>
       </c>
-      <c r="J12" s="18">
+      <c r="J12" s="14">
         <v>5.2999999999999999E-2</v>
       </c>
-      <c r="K12" s="18">
+      <c r="K12" s="14">
         <v>0.81699999999999995</v>
       </c>
-      <c r="L12" s="18">
+      <c r="L12" s="14">
         <v>0.79200000000000004</v>
       </c>
-      <c r="M12" s="18">
+      <c r="M12" s="14">
         <v>352</v>
       </c>
-      <c r="N12" s="19">
+      <c r="N12" s="15">
         <v>6310</v>
       </c>
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A13" s="17">
-        <v>12</v>
-      </c>
-      <c r="B13" s="18" t="s">
+      <c r="A13" s="13">
+        <v>12</v>
+      </c>
+      <c r="B13" s="14" t="s">
         <v>17</v>
       </c>
       <c r="C13" s="2"/>
-      <c r="D13" s="18" t="s">
-        <v>12</v>
-      </c>
-      <c r="E13" s="18" t="s">
-        <v>12</v>
-      </c>
-      <c r="F13" s="18" t="s">
+      <c r="D13" s="14" t="s">
+        <v>12</v>
+      </c>
+      <c r="E13" s="14" t="s">
+        <v>12</v>
+      </c>
+      <c r="F13" s="14" t="s">
         <v>16</v>
       </c>
-      <c r="G13" s="18">
+      <c r="G13" s="14">
         <v>0.5</v>
       </c>
-      <c r="H13" s="18">
+      <c r="H13" s="14">
         <v>0.80700000000000005</v>
       </c>
-      <c r="I13" s="18">
+      <c r="I13" s="14">
         <v>0.48</v>
       </c>
-      <c r="J13" s="18">
+      <c r="J13" s="14">
         <v>0.06</v>
       </c>
-      <c r="K13" s="18">
+      <c r="K13" s="14">
         <v>0.78900000000000003</v>
       </c>
-      <c r="L13" s="18">
+      <c r="L13" s="14">
         <v>0.82499999999999996</v>
       </c>
-      <c r="M13" s="18">
+      <c r="M13" s="14">
         <v>340</v>
       </c>
-      <c r="N13" s="19">
+      <c r="N13" s="15">
         <v>5298</v>
       </c>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A14" s="14">
+      <c r="A14" s="13">
         <v>13</v>
       </c>
       <c r="B14" s="2" t="s">
@@ -4289,12 +4290,12 @@
       <c r="M14" s="2">
         <v>337</v>
       </c>
-      <c r="N14" s="15">
+      <c r="N14" s="11">
         <v>7231</v>
       </c>
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A15" s="14">
+      <c r="A15" s="13">
         <v>14</v>
       </c>
       <c r="B15" s="2" t="s">
@@ -4331,12 +4332,12 @@
       <c r="M15" s="2">
         <v>339</v>
       </c>
-      <c r="N15" s="15">
+      <c r="N15" s="11">
         <v>7101</v>
       </c>
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A16" s="14">
+      <c r="A16" s="13">
         <v>15</v>
       </c>
       <c r="B16" s="2" t="s">
@@ -4373,15 +4374,15 @@
       <c r="M16" s="2">
         <v>349</v>
       </c>
-      <c r="N16" s="15">
+      <c r="N16" s="11">
         <v>5882</v>
       </c>
     </row>
     <row r="17" spans="1:14" ht="75" x14ac:dyDescent="0.25">
-      <c r="A17" s="14">
-        <v>18</v>
-      </c>
-      <c r="B17" s="16" t="s">
+      <c r="A17" s="13">
+        <v>16</v>
+      </c>
+      <c r="B17" s="12" t="s">
         <v>28</v>
       </c>
       <c r="C17" s="2"/>
@@ -4415,126 +4416,126 @@
       <c r="M17" s="2">
         <v>351</v>
       </c>
-      <c r="N17" s="15">
+      <c r="N17" s="11">
         <v>6426</v>
       </c>
     </row>
     <row r="18" spans="1:14" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="27">
-        <v>21</v>
-      </c>
-      <c r="B18" s="28" t="s">
+      <c r="A18" s="31">
+        <v>17</v>
+      </c>
+      <c r="B18" s="24" t="s">
         <v>29</v>
       </c>
-      <c r="C18" s="29"/>
-      <c r="D18" s="29" t="s">
-        <v>12</v>
-      </c>
-      <c r="E18" s="29" t="s">
-        <v>13</v>
-      </c>
-      <c r="F18" s="29" t="s">
-        <v>14</v>
-      </c>
-      <c r="G18" s="29">
+      <c r="C18" s="25"/>
+      <c r="D18" s="25" t="s">
+        <v>12</v>
+      </c>
+      <c r="E18" s="25" t="s">
+        <v>13</v>
+      </c>
+      <c r="F18" s="25" t="s">
+        <v>14</v>
+      </c>
+      <c r="G18" s="25">
         <v>0.5</v>
       </c>
-      <c r="H18" s="29">
+      <c r="H18" s="25">
         <v>0.81299999999999994</v>
       </c>
-      <c r="I18" s="29">
+      <c r="I18" s="25">
         <v>0.46</v>
       </c>
-      <c r="J18" s="29">
+      <c r="J18" s="25">
         <v>6.0999999999999999E-2</v>
       </c>
-      <c r="K18" s="29">
+      <c r="K18" s="25">
         <v>0.8</v>
       </c>
-      <c r="L18" s="29">
+      <c r="L18" s="25">
         <v>0.82399999999999995</v>
       </c>
-      <c r="M18" s="29">
+      <c r="M18" s="25">
         <v>345</v>
       </c>
-      <c r="N18" s="30">
+      <c r="N18" s="26">
         <v>5314</v>
       </c>
     </row>
     <row r="19" spans="1:14" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="4" t="s">
+      <c r="A19" s="27" t="s">
         <v>20</v>
       </c>
-      <c r="B19" s="5"/>
-      <c r="C19" s="5"/>
-      <c r="D19" s="5"/>
-      <c r="E19" s="5"/>
-      <c r="F19" s="5"/>
-      <c r="G19" s="5"/>
-      <c r="H19" s="6">
+      <c r="B19" s="28"/>
+      <c r="C19" s="28"/>
+      <c r="D19" s="28"/>
+      <c r="E19" s="28"/>
+      <c r="F19" s="28"/>
+      <c r="G19" s="28"/>
+      <c r="H19" s="4">
         <f>AVERAGE(H2:H18)</f>
         <v>0.79517647058823548</v>
       </c>
-      <c r="I19" s="6">
+      <c r="I19" s="4">
         <f t="shared" ref="I19:N19" si="0">AVERAGE(I2:I18)</f>
         <v>0.30352941176470588</v>
       </c>
-      <c r="J19" s="6">
+      <c r="J19" s="4">
         <f t="shared" si="0"/>
         <v>5.2882352941176484E-2</v>
       </c>
-      <c r="K19" s="6">
+      <c r="K19" s="4">
         <f t="shared" si="0"/>
         <v>0.79517647058823537</v>
       </c>
-      <c r="L19" s="6">
+      <c r="L19" s="4">
         <f t="shared" si="0"/>
         <v>0.79170588235294126</v>
       </c>
-      <c r="M19" s="7">
+      <c r="M19" s="5">
         <f t="shared" si="0"/>
         <v>342.70588235294116</v>
       </c>
-      <c r="N19" s="8">
+      <c r="N19" s="6">
         <f t="shared" si="0"/>
         <v>6207.6470588235297</v>
       </c>
     </row>
     <row r="20" spans="1:14" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="9" t="s">
+      <c r="A20" s="29" t="s">
         <v>21</v>
       </c>
-      <c r="B20" s="10"/>
-      <c r="C20" s="10"/>
-      <c r="D20" s="10"/>
-      <c r="E20" s="10"/>
-      <c r="F20" s="10"/>
-      <c r="G20" s="10"/>
-      <c r="H20" s="11">
+      <c r="B20" s="30"/>
+      <c r="C20" s="30"/>
+      <c r="D20" s="30"/>
+      <c r="E20" s="30"/>
+      <c r="F20" s="30"/>
+      <c r="G20" s="30"/>
+      <c r="H20" s="7">
         <f>_xlfn.STDEV.P(H2:H18)</f>
         <v>1.4697880175756631E-2</v>
       </c>
-      <c r="I20" s="11">
+      <c r="I20" s="7">
         <f t="shared" ref="I20:N20" si="1">_xlfn.STDEV.P(I2:I18)</f>
         <v>0.17931048250157627</v>
       </c>
-      <c r="J20" s="11">
+      <c r="J20" s="7">
         <f t="shared" si="1"/>
         <v>4.9215295678475025E-3</v>
       </c>
-      <c r="K20" s="11">
+      <c r="K20" s="7">
         <f t="shared" si="1"/>
         <v>2.4588938914784763E-2</v>
       </c>
-      <c r="L20" s="11">
+      <c r="L20" s="7">
         <f t="shared" si="1"/>
         <v>2.7970077931882331E-2</v>
       </c>
-      <c r="M20" s="12">
+      <c r="M20" s="8">
         <f t="shared" si="1"/>
         <v>10.598361171217508</v>
       </c>
-      <c r="N20" s="13">
+      <c r="N20" s="9">
         <f t="shared" si="1"/>
         <v>618.13123879456407</v>
       </c>

</xml_diff>